<commit_message>
Kinda working now. Needs some testing.. and probably some textures :o
</commit_message>
<xml_diff>
--- a/Mappe1.xlsx
+++ b/Mappe1.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MCModDev\1.7\ODIB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13605"/>
   </bookViews>
@@ -12,9 +17,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$A$638</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -411,8 +416,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -715,21 +720,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N127"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I100" workbookViewId="0">
-      <selection activeCell="L127" sqref="L127"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="S127" sqref="S1:S127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="88.140625" bestFit="1" customWidth="1"/>
@@ -737,9 +742,10 @@
     <col min="8" max="8" width="46.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="47" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="109.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="47.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -773,8 +779,12 @@
         <f>CONCATENATE("public static boolean ",A1," = false;")</f>
         <v>public static boolean Adamantium = false;</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="S1" t="str">
+        <f>CONCATENATE("tile.block",A1,".name=Block of ",A1)</f>
+        <v>tile.blockAdamantium.name=Block of Adamantium</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -798,15 +808,19 @@
         <v>copy dummy.png Block_Aluminium.png</v>
       </c>
       <c r="L2" t="str">
-        <f t="shared" ref="L2:N65" si="4">CONCATENATE("public static boolean ",A2," = config.get(",$B$1,"enabledBlocks",$B$1,", ",$B$1,"",A2,$B$1,", true).getBoolean(true);")</f>
+        <f t="shared" ref="L2:L65" si="4">CONCATENATE("public static boolean ",A2," = config.get(",$B$1,"enabledBlocks",$B$1,", ",$B$1,"",A2,$B$1,", true).getBoolean(true);")</f>
         <v>public static boolean Aluminium = config.get("enabledBlocks", "Aluminium", true).getBoolean(true);</v>
       </c>
       <c r="N2" t="str">
         <f t="shared" ref="N2:N65" si="5">CONCATENATE("public static boolean ",A2," = false;")</f>
         <v>public static boolean Aluminium = false;</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="S2" t="str">
+        <f t="shared" ref="S2:S65" si="6">CONCATENATE("tile.block",A2,".name=Block of ",A2)</f>
+        <v>tile.blockAluminium.name=Block of Aluminium</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -837,8 +851,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Americium = false;</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="S3" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockAmericium.name=Block of Americium</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -869,8 +887,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean AnnealedCopper = false;</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="S4" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockAnnealedCopper.name=Block of AnnealedCopper</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -901,8 +923,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Antimony = false;</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="S5" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockAntimony.name=Block of Antimony</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -933,8 +959,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean AstralSilver = false;</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="S6" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockAstralSilver.name=Block of AstralSilver</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -965,8 +995,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean BatteryAlloy = false;</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="S7" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockBatteryAlloy.name=Block of BatteryAlloy</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -997,8 +1031,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Beryllium = false;</v>
       </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="S8" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockBeryllium.name=Block of Beryllium</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1029,8 +1067,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean BismuthBronze = false;</v>
       </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="S9" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockBismuthBronze.name=Block of BismuthBronze</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1061,8 +1103,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Bismuth = false;</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="S10" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockBismuth.name=Block of Bismuth</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1093,8 +1139,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean BlackBronze = false;</v>
       </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="S11" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockBlackBronze.name=Block of BlackBronze</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1125,8 +1175,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean BlackSteel = false;</v>
       </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="S12" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockBlackSteel.name=Block of BlackSteel</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1157,8 +1211,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean BlueAlloy = false;</v>
       </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="S13" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockBlueAlloy.name=Block of BlueAlloy</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1189,8 +1247,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean BlueSteel = false;</v>
       </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="S14" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockBlueSteel.name=Block of BlueSteel</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1221,8 +1283,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Brass = false;</v>
       </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="S15" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockBrass.name=Block of Brass</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1253,8 +1319,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Bronze = false;</v>
       </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="S16" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockBronze.name=Block of Bronze</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1285,8 +1355,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Caesium = false;</v>
       </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="S17" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockCaesium.name=Block of Caesium</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1317,8 +1391,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Cerium = false;</v>
       </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="S18" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockCerium.name=Block of Cerium</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1349,8 +1427,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Chrome = false;</v>
       </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="S19" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockChrome.name=Block of Chrome</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1381,8 +1463,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean ChromiumDioxide = false;</v>
       </c>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="S20" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockChromiumDioxide.name=Block of ChromiumDioxide</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1413,8 +1499,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean CobaltBrass = false;</v>
       </c>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="S21" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockCobaltBrass.name=Block of CobaltBrass</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1445,8 +1535,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Cobalt = false;</v>
       </c>
-    </row>
-    <row r="23" spans="1:14">
+      <c r="S22" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockCobalt.name=Block of Cobalt</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1477,8 +1571,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Copper = false;</v>
       </c>
-    </row>
-    <row r="24" spans="1:14">
+      <c r="S23" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockCopper.name=Block of Copper</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1509,8 +1607,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Cupronickel = false;</v>
       </c>
-    </row>
-    <row r="25" spans="1:14">
+      <c r="S24" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockCupronickel.name=Block of Cupronickel</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1541,8 +1643,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean DamascusSteel = false;</v>
       </c>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="S25" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockDamascusSteel.name=Block of DamascusSteel</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1573,8 +1679,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean DarkIron = false;</v>
       </c>
-    </row>
-    <row r="27" spans="1:14">
+      <c r="S26" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockDarkIron.name=Block of DarkIron</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1605,8 +1715,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean DeepIron = false;</v>
       </c>
-    </row>
-    <row r="28" spans="1:14">
+      <c r="S27" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockDeepIron.name=Block of DeepIron</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1637,8 +1751,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Desh = false;</v>
       </c>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="S28" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockDesh.name=Block of Desh</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1669,8 +1787,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Duranium = false;</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="S29" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockDuranium.name=Block of Duranium</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1701,8 +1823,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Dysprosium = false;</v>
       </c>
-    </row>
-    <row r="31" spans="1:14">
+      <c r="S30" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockDysprosium.name=Block of Dysprosium</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1733,8 +1859,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean ElectrumFlux = false;</v>
       </c>
-    </row>
-    <row r="32" spans="1:14">
+      <c r="S31" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockElectrumFlux.name=Block of ElectrumFlux</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1765,8 +1895,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Electrum = false;</v>
       </c>
-    </row>
-    <row r="33" spans="1:14">
+      <c r="S32" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockElectrum.name=Block of Electrum</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1797,8 +1931,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Enderium = false;</v>
       </c>
-    </row>
-    <row r="34" spans="1:14">
+      <c r="S33" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockEnderium.name=Block of Enderium</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1829,8 +1967,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Erbium = false;</v>
       </c>
-    </row>
-    <row r="35" spans="1:14">
+      <c r="S34" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockErbium.name=Block of Erbium</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1861,8 +2003,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Europium = false;</v>
       </c>
-    </row>
-    <row r="36" spans="1:14">
+      <c r="S35" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockEuropium.name=Block of Europium</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1893,8 +2039,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean FierySteel = false;</v>
       </c>
-    </row>
-    <row r="37" spans="1:14">
+      <c r="S36" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockFierySteel.name=Block of FierySteel</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1925,8 +2075,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Force = false;</v>
       </c>
-    </row>
-    <row r="38" spans="1:14">
+      <c r="S37" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockForce.name=Block of Force</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1957,8 +2111,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Gadolinium = false;</v>
       </c>
-    </row>
-    <row r="39" spans="1:14">
+      <c r="S38" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockGadolinium.name=Block of Gadolinium</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1989,8 +2147,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Gallium = false;</v>
       </c>
-    </row>
-    <row r="40" spans="1:14">
+      <c r="S39" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockGallium.name=Block of Gallium</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2021,8 +2183,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Gold = false;</v>
       </c>
-    </row>
-    <row r="41" spans="1:14">
+      <c r="S40" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockGold.name=Block of Gold</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2053,8 +2219,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean HSLA = false;</v>
       </c>
-    </row>
-    <row r="42" spans="1:14">
+      <c r="S41" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockHSLA.name=Block of HSLA</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2085,8 +2255,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Holmium = false;</v>
       </c>
-    </row>
-    <row r="43" spans="1:14">
+      <c r="S42" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockHolmium.name=Block of Holmium</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -2117,8 +2291,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Indium = false;</v>
       </c>
-    </row>
-    <row r="44" spans="1:14">
+      <c r="S43" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockIndium.name=Block of Indium</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -2149,8 +2327,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean InfusedGold = false;</v>
       </c>
-    </row>
-    <row r="45" spans="1:14">
+      <c r="S44" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockInfusedGold.name=Block of InfusedGold</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2181,8 +2363,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Invar = false;</v>
       </c>
-    </row>
-    <row r="46" spans="1:14">
+      <c r="S45" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockInvar.name=Block of Invar</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2213,8 +2399,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Iridium = false;</v>
       </c>
-    </row>
-    <row r="47" spans="1:14">
+      <c r="S46" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockIridium.name=Block of Iridium</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2245,8 +2435,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean IronMagnetic = false;</v>
       </c>
-    </row>
-    <row r="48" spans="1:14">
+      <c r="S47" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockIronMagnetic.name=Block of IronMagnetic</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -2277,8 +2471,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean IronWood = false;</v>
       </c>
-    </row>
-    <row r="49" spans="1:14">
+      <c r="S48" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockIronWood.name=Block of IronWood</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -2309,8 +2507,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Iron = false;</v>
       </c>
-    </row>
-    <row r="50" spans="1:14">
+      <c r="S49" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockIron.name=Block of Iron</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -2341,8 +2543,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Kanthal = false;</v>
       </c>
-    </row>
-    <row r="51" spans="1:14">
+      <c r="S50" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockKanthal.name=Block of Kanthal</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -2373,8 +2579,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Knightmetal = false;</v>
       </c>
-    </row>
-    <row r="52" spans="1:14">
+      <c r="S51" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockKnightmetal.name=Block of Knightmetal</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -2405,8 +2615,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Lanthanum = false;</v>
       </c>
-    </row>
-    <row r="53" spans="1:14">
+      <c r="S52" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockLanthanum.name=Block of Lanthanum</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2437,8 +2651,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Lead = false;</v>
       </c>
-    </row>
-    <row r="54" spans="1:14">
+      <c r="S53" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockLead.name=Block of Lead</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2469,8 +2687,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Lutetium = false;</v>
       </c>
-    </row>
-    <row r="55" spans="1:14">
+      <c r="S54" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockLutetium.name=Block of Lutetium</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2501,8 +2723,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Magnalium = false;</v>
       </c>
-    </row>
-    <row r="56" spans="1:14">
+      <c r="S55" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockMagnalium.name=Block of Magnalium</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2533,8 +2759,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Magnesium = false;</v>
       </c>
-    </row>
-    <row r="57" spans="1:14">
+      <c r="S56" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockMagnesium.name=Block of Magnesium</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -2565,8 +2795,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Manganese = false;</v>
       </c>
-    </row>
-    <row r="58" spans="1:14">
+      <c r="S57" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockManganese.name=Block of Manganese</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -2597,8 +2831,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean MeteoricIron = false;</v>
       </c>
-    </row>
-    <row r="59" spans="1:14">
+      <c r="S58" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockMeteoricIron.name=Block of MeteoricIron</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -2629,8 +2867,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean MeteoricSteel = false;</v>
       </c>
-    </row>
-    <row r="60" spans="1:14">
+      <c r="S59" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockMeteoricSteel.name=Block of MeteoricSteel</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -2661,8 +2903,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Midasium = false;</v>
       </c>
-    </row>
-    <row r="61" spans="1:14">
+      <c r="S60" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockMidasium.name=Block of Midasium</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>62</v>
       </c>
@@ -2693,8 +2939,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Mithril = false;</v>
       </c>
-    </row>
-    <row r="62" spans="1:14">
+      <c r="S61" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockMithril.name=Block of Mithril</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -2725,8 +2975,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Molybdenum = false;</v>
       </c>
-    </row>
-    <row r="63" spans="1:14">
+      <c r="S62" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockMolybdenum.name=Block of Molybdenum</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -2757,8 +3011,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean NaquadahAlloy = false;</v>
       </c>
-    </row>
-    <row r="64" spans="1:14">
+      <c r="S63" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockNaquadahAlloy.name=Block of NaquadahAlloy</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -2789,8 +3047,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean NaquadahEnriched = false;</v>
       </c>
-    </row>
-    <row r="65" spans="1:14">
+      <c r="S64" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockNaquadahEnriched.name=Block of NaquadahEnriched</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -2821,8 +3083,12 @@
         <f t="shared" si="5"/>
         <v>public static boolean Naquadah = false;</v>
       </c>
-    </row>
-    <row r="66" spans="1:14">
+      <c r="S65" t="str">
+        <f t="shared" si="6"/>
+        <v>tile.blockNaquadah.name=Block of Naquadah</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -2830,31 +3096,35 @@
         <v>66</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" ref="D66:D127" si="6">CONCATENATE("public static Block _",A66,"Block = new BlockBase(",$B$1,"block",A66,$B$1,");")</f>
+        <f t="shared" ref="D66:D127" si="7">CONCATENATE("public static Block _",A66,"Block = new BlockBase(",$B$1,"block",A66,$B$1,");")</f>
         <v>public static Block _NaquadriaBlock = new BlockBase("blockNaquadria");</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" ref="F66:F127" si="7">CONCATENATE("OreDictionary.registerOre(",$B$1,"block",A66,$B$1,", new ItemStack(_",A66,"Block, 1, ",C66,"));")</f>
+        <f t="shared" ref="F66:F127" si="8">CONCATENATE("OreDictionary.registerOre(",$B$1,"block",A66,$B$1,", new ItemStack(_",A66,"Block, 1, ",C66,"));")</f>
         <v>OreDictionary.registerOre("blockNaquadria", new ItemStack(_NaquadriaBlock, 1, 66));</v>
       </c>
       <c r="H66" t="str">
-        <f t="shared" ref="H66:H127" si="8">CONCATENATE("RegisterHelper.registerBlock(_",A66,"Block);")</f>
+        <f t="shared" ref="H66:H127" si="9">CONCATENATE("RegisterHelper.registerBlock(_",A66,"Block);")</f>
         <v>RegisterHelper.registerBlock(_NaquadriaBlock);</v>
       </c>
       <c r="K66" t="str">
-        <f t="shared" ref="K66:K127" si="9">CONCATENATE("copy dummy.png Block_",A66,".png")</f>
+        <f t="shared" ref="K66:K127" si="10">CONCATENATE("copy dummy.png Block_",A66,".png")</f>
         <v>copy dummy.png Block_Naquadria.png</v>
       </c>
       <c r="L66" t="str">
-        <f t="shared" ref="L66:N127" si="10">CONCATENATE("public static boolean ",A66," = config.get(",$B$1,"enabledBlocks",$B$1,", ",$B$1,"",A66,$B$1,", true).getBoolean(true);")</f>
+        <f t="shared" ref="L66:L127" si="11">CONCATENATE("public static boolean ",A66," = config.get(",$B$1,"enabledBlocks",$B$1,", ",$B$1,"",A66,$B$1,", true).getBoolean(true);")</f>
         <v>public static boolean Naquadria = config.get("enabledBlocks", "Naquadria", true).getBoolean(true);</v>
       </c>
       <c r="N66" t="str">
-        <f t="shared" ref="N66:N127" si="11">CONCATENATE("public static boolean ",A66," = false;")</f>
+        <f t="shared" ref="N66:N127" si="12">CONCATENATE("public static boolean ",A66," = false;")</f>
         <v>public static boolean Naquadria = false;</v>
       </c>
-    </row>
-    <row r="67" spans="1:14">
+      <c r="S66" t="str">
+        <f t="shared" ref="S66:S127" si="13">CONCATENATE("tile.block",A66,".name=Block of ",A66)</f>
+        <v>tile.blockNaquadria.name=Block of Naquadria</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>68</v>
       </c>
@@ -2862,31 +3132,35 @@
         <v>67</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _NeodymiumMagneticBlock = new BlockBase("blockNeodymiumMagnetic");</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockNeodymiumMagnetic", new ItemStack(_NeodymiumMagneticBlock, 1, 67));</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_NeodymiumMagneticBlock);</v>
       </c>
       <c r="K67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_NeodymiumMagnetic.png</v>
       </c>
       <c r="L67" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean NeodymiumMagnetic = config.get("enabledBlocks", "NeodymiumMagnetic", true).getBoolean(true);</v>
       </c>
       <c r="N67" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean NeodymiumMagnetic = false;</v>
       </c>
-    </row>
-    <row r="68" spans="1:14">
+      <c r="S67" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockNeodymiumMagnetic.name=Block of NeodymiumMagnetic</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>69</v>
       </c>
@@ -2894,31 +3168,35 @@
         <v>68</v>
       </c>
       <c r="D68" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _NeodymiumBlock = new BlockBase("blockNeodymium");</v>
       </c>
       <c r="F68" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockNeodymium", new ItemStack(_NeodymiumBlock, 1, 68));</v>
       </c>
       <c r="H68" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_NeodymiumBlock);</v>
       </c>
       <c r="K68" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Neodymium.png</v>
       </c>
       <c r="L68" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Neodymium = config.get("enabledBlocks", "Neodymium", true).getBoolean(true);</v>
       </c>
       <c r="N68" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Neodymium = false;</v>
       </c>
-    </row>
-    <row r="69" spans="1:14">
+      <c r="S68" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockNeodymium.name=Block of Neodymium</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -2926,31 +3204,35 @@
         <v>69</v>
       </c>
       <c r="D69" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _NeutroniumBlock = new BlockBase("blockNeutronium");</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockNeutronium", new ItemStack(_NeutroniumBlock, 1, 69));</v>
       </c>
       <c r="H69" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_NeutroniumBlock);</v>
       </c>
       <c r="K69" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Neutronium.png</v>
       </c>
       <c r="L69" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Neutronium = config.get("enabledBlocks", "Neutronium", true).getBoolean(true);</v>
       </c>
       <c r="N69" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Neutronium = false;</v>
       </c>
-    </row>
-    <row r="70" spans="1:14">
+      <c r="S69" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockNeutronium.name=Block of Neutronium</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>71</v>
       </c>
@@ -2958,31 +3240,35 @@
         <v>70</v>
       </c>
       <c r="D70" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _NichromeBlock = new BlockBase("blockNichrome");</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockNichrome", new ItemStack(_NichromeBlock, 1, 70));</v>
       </c>
       <c r="H70" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_NichromeBlock);</v>
       </c>
       <c r="K70" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Nichrome.png</v>
       </c>
       <c r="L70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Nichrome = config.get("enabledBlocks", "Nichrome", true).getBoolean(true);</v>
       </c>
       <c r="N70" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Nichrome = false;</v>
       </c>
-    </row>
-    <row r="71" spans="1:14">
+      <c r="S70" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockNichrome.name=Block of Nichrome</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>72</v>
       </c>
@@ -2990,31 +3276,35 @@
         <v>71</v>
       </c>
       <c r="D71" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _NickelBlock = new BlockBase("blockNickel");</v>
       </c>
       <c r="F71" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockNickel", new ItemStack(_NickelBlock, 1, 71));</v>
       </c>
       <c r="H71" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_NickelBlock);</v>
       </c>
       <c r="K71" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Nickel.png</v>
       </c>
       <c r="L71" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Nickel = config.get("enabledBlocks", "Nickel", true).getBoolean(true);</v>
       </c>
       <c r="N71" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Nickel = false;</v>
       </c>
-    </row>
-    <row r="72" spans="1:14">
+      <c r="S71" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockNickel.name=Block of Nickel</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>73</v>
       </c>
@@ -3022,31 +3312,35 @@
         <v>72</v>
       </c>
       <c r="D72" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _NiobiumNitrideBlock = new BlockBase("blockNiobiumNitride");</v>
       </c>
       <c r="F72" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockNiobiumNitride", new ItemStack(_NiobiumNitrideBlock, 1, 72));</v>
       </c>
       <c r="H72" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_NiobiumNitrideBlock);</v>
       </c>
       <c r="K72" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_NiobiumNitride.png</v>
       </c>
       <c r="L72" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean NiobiumNitride = config.get("enabledBlocks", "NiobiumNitride", true).getBoolean(true);</v>
       </c>
       <c r="N72" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean NiobiumNitride = false;</v>
       </c>
-    </row>
-    <row r="73" spans="1:14">
+      <c r="S72" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockNiobiumNitride.name=Block of NiobiumNitride</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>74</v>
       </c>
@@ -3054,31 +3348,35 @@
         <v>73</v>
       </c>
       <c r="D73" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _NiobiumTitaniumBlock = new BlockBase("blockNiobiumTitanium");</v>
       </c>
       <c r="F73" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockNiobiumTitanium", new ItemStack(_NiobiumTitaniumBlock, 1, 73));</v>
       </c>
       <c r="H73" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_NiobiumTitaniumBlock);</v>
       </c>
       <c r="K73" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_NiobiumTitanium.png</v>
       </c>
       <c r="L73" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean NiobiumTitanium = config.get("enabledBlocks", "NiobiumTitanium", true).getBoolean(true);</v>
       </c>
       <c r="N73" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean NiobiumTitanium = false;</v>
       </c>
-    </row>
-    <row r="74" spans="1:14">
+      <c r="S73" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockNiobiumTitanium.name=Block of NiobiumTitanium</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>75</v>
       </c>
@@ -3086,31 +3384,35 @@
         <v>74</v>
       </c>
       <c r="D74" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _NiobiumBlock = new BlockBase("blockNiobium");</v>
       </c>
       <c r="F74" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockNiobium", new ItemStack(_NiobiumBlock, 1, 74));</v>
       </c>
       <c r="H74" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_NiobiumBlock);</v>
       </c>
       <c r="K74" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Niobium.png</v>
       </c>
       <c r="L74" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Niobium = config.get("enabledBlocks", "Niobium", true).getBoolean(true);</v>
       </c>
       <c r="N74" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Niobium = false;</v>
       </c>
-    </row>
-    <row r="75" spans="1:14">
+      <c r="S74" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockNiobium.name=Block of Niobium</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>76</v>
       </c>
@@ -3118,31 +3420,35 @@
         <v>75</v>
       </c>
       <c r="D75" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _OsmiridiumBlock = new BlockBase("blockOsmiridium");</v>
       </c>
       <c r="F75" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockOsmiridium", new ItemStack(_OsmiridiumBlock, 1, 75));</v>
       </c>
       <c r="H75" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_OsmiridiumBlock);</v>
       </c>
       <c r="K75" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Osmiridium.png</v>
       </c>
       <c r="L75" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Osmiridium = config.get("enabledBlocks", "Osmiridium", true).getBoolean(true);</v>
       </c>
       <c r="N75" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Osmiridium = false;</v>
       </c>
-    </row>
-    <row r="76" spans="1:14">
+      <c r="S75" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockOsmiridium.name=Block of Osmiridium</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>77</v>
       </c>
@@ -3150,31 +3456,35 @@
         <v>76</v>
       </c>
       <c r="D76" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _OsmiumBlock = new BlockBase("blockOsmium");</v>
       </c>
       <c r="F76" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockOsmium", new ItemStack(_OsmiumBlock, 1, 76));</v>
       </c>
       <c r="H76" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_OsmiumBlock);</v>
       </c>
       <c r="K76" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Osmium.png</v>
       </c>
       <c r="L76" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Osmium = config.get("enabledBlocks", "Osmium", true).getBoolean(true);</v>
       </c>
       <c r="N76" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Osmium = false;</v>
       </c>
-    </row>
-    <row r="77" spans="1:14">
+      <c r="S76" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockOsmium.name=Block of Osmium</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>78</v>
       </c>
@@ -3182,31 +3492,35 @@
         <v>77</v>
       </c>
       <c r="D77" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _PalladiumBlock = new BlockBase("blockPalladium");</v>
       </c>
       <c r="F77" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockPalladium", new ItemStack(_PalladiumBlock, 1, 77));</v>
       </c>
       <c r="H77" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_PalladiumBlock);</v>
       </c>
       <c r="K77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Palladium.png</v>
       </c>
       <c r="L77" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Palladium = config.get("enabledBlocks", "Palladium", true).getBoolean(true);</v>
       </c>
       <c r="N77" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Palladium = false;</v>
       </c>
-    </row>
-    <row r="78" spans="1:14">
+      <c r="S77" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockPalladium.name=Block of Palladium</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>79</v>
       </c>
@@ -3214,31 +3528,35 @@
         <v>78</v>
       </c>
       <c r="D78" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _PigIronBlock = new BlockBase("blockPigIron");</v>
       </c>
       <c r="F78" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockPigIron", new ItemStack(_PigIronBlock, 1, 78));</v>
       </c>
       <c r="H78" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_PigIronBlock);</v>
       </c>
       <c r="K78" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_PigIron.png</v>
       </c>
       <c r="L78" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean PigIron = config.get("enabledBlocks", "PigIron", true).getBoolean(true);</v>
       </c>
       <c r="N78" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean PigIron = false;</v>
       </c>
-    </row>
-    <row r="79" spans="1:14">
+      <c r="S78" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockPigIron.name=Block of PigIron</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>81</v>
       </c>
@@ -3246,31 +3564,35 @@
         <v>79</v>
       </c>
       <c r="D79" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _PlatinumBlock = new BlockBase("blockPlatinum");</v>
       </c>
       <c r="F79" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockPlatinum", new ItemStack(_PlatinumBlock, 1, 79));</v>
       </c>
       <c r="H79" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_PlatinumBlock);</v>
       </c>
       <c r="K79" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Platinum.png</v>
       </c>
       <c r="L79" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Platinum = config.get("enabledBlocks", "Platinum", true).getBoolean(true);</v>
       </c>
       <c r="N79" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Platinum = false;</v>
       </c>
-    </row>
-    <row r="80" spans="1:14">
+      <c r="S79" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockPlatinum.name=Block of Platinum</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -3278,31 +3600,35 @@
         <v>80</v>
       </c>
       <c r="D80" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _Plutonium241Block = new BlockBase("blockPlutonium241");</v>
       </c>
       <c r="F80" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockPlutonium241", new ItemStack(_Plutonium241Block, 1, 80));</v>
       </c>
       <c r="H80" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_Plutonium241Block);</v>
       </c>
       <c r="K80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Plutonium241.png</v>
       </c>
       <c r="L80" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Plutonium241 = config.get("enabledBlocks", "Plutonium241", true).getBoolean(true);</v>
       </c>
       <c r="N80" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Plutonium241 = false;</v>
       </c>
-    </row>
-    <row r="81" spans="1:14">
+      <c r="S80" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockPlutonium241.name=Block of Plutonium241</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>83</v>
       </c>
@@ -3310,31 +3636,35 @@
         <v>81</v>
       </c>
       <c r="D81" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _PlutoniumBlock = new BlockBase("blockPlutonium");</v>
       </c>
       <c r="F81" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockPlutonium", new ItemStack(_PlutoniumBlock, 1, 81));</v>
       </c>
       <c r="H81" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_PlutoniumBlock);</v>
       </c>
       <c r="K81" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Plutonium.png</v>
       </c>
       <c r="L81" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Plutonium = config.get("enabledBlocks", "Plutonium", true).getBoolean(true);</v>
       </c>
       <c r="N81" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Plutonium = false;</v>
       </c>
-    </row>
-    <row r="82" spans="1:14">
+      <c r="S81" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockPlutonium.name=Block of Plutonium</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>84</v>
       </c>
@@ -3342,31 +3672,35 @@
         <v>82</v>
       </c>
       <c r="D82" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _PraseodymiumBlock = new BlockBase("blockPraseodymium");</v>
       </c>
       <c r="F82" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockPraseodymium", new ItemStack(_PraseodymiumBlock, 1, 82));</v>
       </c>
       <c r="H82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_PraseodymiumBlock);</v>
       </c>
       <c r="K82" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Praseodymium.png</v>
       </c>
       <c r="L82" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Praseodymium = config.get("enabledBlocks", "Praseodymium", true).getBoolean(true);</v>
       </c>
       <c r="N82" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Praseodymium = false;</v>
       </c>
-    </row>
-    <row r="83" spans="1:14">
+      <c r="S82" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockPraseodymium.name=Block of Praseodymium</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>85</v>
       </c>
@@ -3374,31 +3708,35 @@
         <v>83</v>
       </c>
       <c r="D83" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _PromethiumBlock = new BlockBase("blockPromethium");</v>
       </c>
       <c r="F83" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockPromethium", new ItemStack(_PromethiumBlock, 1, 83));</v>
       </c>
       <c r="H83" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_PromethiumBlock);</v>
       </c>
       <c r="K83" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Promethium.png</v>
       </c>
       <c r="L83" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Promethium = config.get("enabledBlocks", "Promethium", true).getBoolean(true);</v>
       </c>
       <c r="N83" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Promethium = false;</v>
       </c>
-    </row>
-    <row r="84" spans="1:14">
+      <c r="S83" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockPromethium.name=Block of Promethium</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>86</v>
       </c>
@@ -3406,31 +3744,35 @@
         <v>84</v>
       </c>
       <c r="D84" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _RedAlloyBlock = new BlockBase("blockRedAlloy");</v>
       </c>
       <c r="F84" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockRedAlloy", new ItemStack(_RedAlloyBlock, 1, 84));</v>
       </c>
       <c r="H84" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_RedAlloyBlock);</v>
       </c>
       <c r="K84" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_RedAlloy.png</v>
       </c>
       <c r="L84" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean RedAlloy = config.get("enabledBlocks", "RedAlloy", true).getBoolean(true);</v>
       </c>
       <c r="N84" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean RedAlloy = false;</v>
       </c>
-    </row>
-    <row r="85" spans="1:14">
+      <c r="S84" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockRedAlloy.name=Block of RedAlloy</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>87</v>
       </c>
@@ -3438,31 +3780,35 @@
         <v>85</v>
       </c>
       <c r="D85" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _RedSteelBlock = new BlockBase("blockRedSteel");</v>
       </c>
       <c r="F85" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockRedSteel", new ItemStack(_RedSteelBlock, 1, 85));</v>
       </c>
       <c r="H85" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_RedSteelBlock);</v>
       </c>
       <c r="K85" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_RedSteel.png</v>
       </c>
       <c r="L85" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean RedSteel = config.get("enabledBlocks", "RedSteel", true).getBoolean(true);</v>
       </c>
       <c r="N85" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean RedSteel = false;</v>
       </c>
-    </row>
-    <row r="86" spans="1:14">
+      <c r="S85" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockRedSteel.name=Block of RedSteel</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>88</v>
       </c>
@@ -3470,31 +3816,35 @@
         <v>86</v>
       </c>
       <c r="D86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _RoseGoldBlock = new BlockBase("blockRoseGold");</v>
       </c>
       <c r="F86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockRoseGold", new ItemStack(_RoseGoldBlock, 1, 86));</v>
       </c>
       <c r="H86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_RoseGoldBlock);</v>
       </c>
       <c r="K86" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_RoseGold.png</v>
       </c>
       <c r="L86" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean RoseGold = config.get("enabledBlocks", "RoseGold", true).getBoolean(true);</v>
       </c>
       <c r="N86" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean RoseGold = false;</v>
       </c>
-    </row>
-    <row r="87" spans="1:14">
+      <c r="S86" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockRoseGold.name=Block of RoseGold</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>90</v>
       </c>
@@ -3502,31 +3852,35 @@
         <v>87</v>
       </c>
       <c r="D87" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _RubidiumBlock = new BlockBase("blockRubidium");</v>
       </c>
       <c r="F87" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockRubidium", new ItemStack(_RubidiumBlock, 1, 87));</v>
       </c>
       <c r="H87" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_RubidiumBlock);</v>
       </c>
       <c r="K87" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Rubidium.png</v>
       </c>
       <c r="L87" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Rubidium = config.get("enabledBlocks", "Rubidium", true).getBoolean(true);</v>
       </c>
       <c r="N87" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Rubidium = false;</v>
       </c>
-    </row>
-    <row r="88" spans="1:14">
+      <c r="S87" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockRubidium.name=Block of Rubidium</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>91</v>
       </c>
@@ -3534,31 +3888,35 @@
         <v>88</v>
       </c>
       <c r="D88" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _SamariumBlock = new BlockBase("blockSamarium");</v>
       </c>
       <c r="F88" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockSamarium", new ItemStack(_SamariumBlock, 1, 88));</v>
       </c>
       <c r="H88" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_SamariumBlock);</v>
       </c>
       <c r="K88" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Samarium.png</v>
       </c>
       <c r="L88" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Samarium = config.get("enabledBlocks", "Samarium", true).getBoolean(true);</v>
       </c>
       <c r="N88" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Samarium = false;</v>
       </c>
-    </row>
-    <row r="89" spans="1:14">
+      <c r="S88" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockSamarium.name=Block of Samarium</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>92</v>
       </c>
@@ -3566,31 +3924,35 @@
         <v>89</v>
       </c>
       <c r="D89" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _ScandiumBlock = new BlockBase("blockScandium");</v>
       </c>
       <c r="F89" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockScandium", new ItemStack(_ScandiumBlock, 1, 89));</v>
       </c>
       <c r="H89" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_ScandiumBlock);</v>
       </c>
       <c r="K89" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Scandium.png</v>
       </c>
       <c r="L89" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Scandium = config.get("enabledBlocks", "Scandium", true).getBoolean(true);</v>
       </c>
       <c r="N89" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Scandium = false;</v>
       </c>
-    </row>
-    <row r="90" spans="1:14">
+      <c r="S89" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockScandium.name=Block of Scandium</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>93</v>
       </c>
@@ -3598,31 +3960,35 @@
         <v>90</v>
       </c>
       <c r="D90" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _ShadowIronBlock = new BlockBase("blockShadowIron");</v>
       </c>
       <c r="F90" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockShadowIron", new ItemStack(_ShadowIronBlock, 1, 90));</v>
       </c>
       <c r="H90" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_ShadowIronBlock);</v>
       </c>
       <c r="K90" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_ShadowIron.png</v>
       </c>
       <c r="L90" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean ShadowIron = config.get("enabledBlocks", "ShadowIron", true).getBoolean(true);</v>
       </c>
       <c r="N90" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean ShadowIron = false;</v>
       </c>
-    </row>
-    <row r="91" spans="1:14">
+      <c r="S90" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockShadowIron.name=Block of ShadowIron</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>94</v>
       </c>
@@ -3630,31 +3996,35 @@
         <v>91</v>
       </c>
       <c r="D91" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _ShadowSteelBlock = new BlockBase("blockShadowSteel");</v>
       </c>
       <c r="F91" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockShadowSteel", new ItemStack(_ShadowSteelBlock, 1, 91));</v>
       </c>
       <c r="H91" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_ShadowSteelBlock);</v>
       </c>
       <c r="K91" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_ShadowSteel.png</v>
       </c>
       <c r="L91" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean ShadowSteel = config.get("enabledBlocks", "ShadowSteel", true).getBoolean(true);</v>
       </c>
       <c r="N91" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean ShadowSteel = false;</v>
       </c>
-    </row>
-    <row r="92" spans="1:14">
+      <c r="S91" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockShadowSteel.name=Block of ShadowSteel</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -3662,31 +4032,35 @@
         <v>92</v>
       </c>
       <c r="D92" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _SiliconBlock = new BlockBase("blockSilicon");</v>
       </c>
       <c r="F92" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockSilicon", new ItemStack(_SiliconBlock, 1, 92));</v>
       </c>
       <c r="H92" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_SiliconBlock);</v>
       </c>
       <c r="K92" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Silicon.png</v>
       </c>
       <c r="L92" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Silicon = config.get("enabledBlocks", "Silicon", true).getBoolean(true);</v>
       </c>
       <c r="N92" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Silicon = false;</v>
       </c>
-    </row>
-    <row r="93" spans="1:14">
+      <c r="S92" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockSilicon.name=Block of Silicon</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>96</v>
       </c>
@@ -3694,31 +4068,35 @@
         <v>93</v>
       </c>
       <c r="D93" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _SilverBlock = new BlockBase("blockSilver");</v>
       </c>
       <c r="F93" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockSilver", new ItemStack(_SilverBlock, 1, 93));</v>
       </c>
       <c r="H93" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_SilverBlock);</v>
       </c>
       <c r="K93" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Silver.png</v>
       </c>
       <c r="L93" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Silver = config.get("enabledBlocks", "Silver", true).getBoolean(true);</v>
       </c>
       <c r="N93" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Silver = false;</v>
       </c>
-    </row>
-    <row r="94" spans="1:14">
+      <c r="S93" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockSilver.name=Block of Silver</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>97</v>
       </c>
@@ -3726,31 +4104,35 @@
         <v>94</v>
       </c>
       <c r="D94" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _SolderingAlloyBlock = new BlockBase("blockSolderingAlloy");</v>
       </c>
       <c r="F94" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockSolderingAlloy", new ItemStack(_SolderingAlloyBlock, 1, 94));</v>
       </c>
       <c r="H94" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_SolderingAlloyBlock);</v>
       </c>
       <c r="K94" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_SolderingAlloy.png</v>
       </c>
       <c r="L94" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean SolderingAlloy = config.get("enabledBlocks", "SolderingAlloy", true).getBoolean(true);</v>
       </c>
       <c r="N94" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean SolderingAlloy = false;</v>
       </c>
-    </row>
-    <row r="95" spans="1:14">
+      <c r="S94" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockSolderingAlloy.name=Block of SolderingAlloy</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>98</v>
       </c>
@@ -3758,31 +4140,35 @@
         <v>95</v>
       </c>
       <c r="D95" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _StainlessSteelBlock = new BlockBase("blockStainlessSteel");</v>
       </c>
       <c r="F95" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockStainlessSteel", new ItemStack(_StainlessSteelBlock, 1, 95));</v>
       </c>
       <c r="H95" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_StainlessSteelBlock);</v>
       </c>
       <c r="K95" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_StainlessSteel.png</v>
       </c>
       <c r="L95" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean StainlessSteel = config.get("enabledBlocks", "StainlessSteel", true).getBoolean(true);</v>
       </c>
       <c r="N95" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean StainlessSteel = false;</v>
       </c>
-    </row>
-    <row r="96" spans="1:14">
+      <c r="S95" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockStainlessSteel.name=Block of StainlessSteel</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>100</v>
       </c>
@@ -3790,31 +4176,35 @@
         <v>96</v>
       </c>
       <c r="D96" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _SteelMagneticBlock = new BlockBase("blockSteelMagnetic");</v>
       </c>
       <c r="F96" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockSteelMagnetic", new ItemStack(_SteelMagneticBlock, 1, 96));</v>
       </c>
       <c r="H96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_SteelMagneticBlock);</v>
       </c>
       <c r="K96" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_SteelMagnetic.png</v>
       </c>
       <c r="L96" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean SteelMagnetic = config.get("enabledBlocks", "SteelMagnetic", true).getBoolean(true);</v>
       </c>
       <c r="N96" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean SteelMagnetic = false;</v>
       </c>
-    </row>
-    <row r="97" spans="1:14">
+      <c r="S96" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockSteelMagnetic.name=Block of SteelMagnetic</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>101</v>
       </c>
@@ -3822,31 +4212,35 @@
         <v>97</v>
       </c>
       <c r="D97" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _SteelBlock = new BlockBase("blockSteel");</v>
       </c>
       <c r="F97" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockSteel", new ItemStack(_SteelBlock, 1, 97));</v>
       </c>
       <c r="H97" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_SteelBlock);</v>
       </c>
       <c r="K97" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Steel.png</v>
       </c>
       <c r="L97" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Steel = config.get("enabledBlocks", "Steel", true).getBoolean(true);</v>
       </c>
       <c r="N97" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Steel = false;</v>
       </c>
-    </row>
-    <row r="98" spans="1:14">
+      <c r="S97" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockSteel.name=Block of Steel</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>102</v>
       </c>
@@ -3854,31 +4248,35 @@
         <v>98</v>
       </c>
       <c r="D98" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _SteeleafBlock = new BlockBase("blockSteeleaf");</v>
       </c>
       <c r="F98" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockSteeleaf", new ItemStack(_SteeleafBlock, 1, 98));</v>
       </c>
       <c r="H98" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_SteeleafBlock);</v>
       </c>
       <c r="K98" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Steeleaf.png</v>
       </c>
       <c r="L98" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Steeleaf = config.get("enabledBlocks", "Steeleaf", true).getBoolean(true);</v>
       </c>
       <c r="N98" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Steeleaf = false;</v>
       </c>
-    </row>
-    <row r="99" spans="1:14">
+      <c r="S98" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockSteeleaf.name=Block of Steeleaf</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>103</v>
       </c>
@@ -3886,31 +4284,35 @@
         <v>99</v>
       </c>
       <c r="D99" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _SterlingSilverBlock = new BlockBase("blockSterlingSilver");</v>
       </c>
       <c r="F99" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockSterlingSilver", new ItemStack(_SterlingSilverBlock, 1, 99));</v>
       </c>
       <c r="H99" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_SterlingSilverBlock);</v>
       </c>
       <c r="K99" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_SterlingSilver.png</v>
       </c>
       <c r="L99" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean SterlingSilver = config.get("enabledBlocks", "SterlingSilver", true).getBoolean(true);</v>
       </c>
       <c r="N99" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean SterlingSilver = false;</v>
       </c>
-    </row>
-    <row r="100" spans="1:14">
+      <c r="S99" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockSterlingSilver.name=Block of SterlingSilver</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>104</v>
       </c>
@@ -3918,31 +4320,35 @@
         <v>100</v>
       </c>
       <c r="D100" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _SunnariumBlock = new BlockBase("blockSunnarium");</v>
       </c>
       <c r="F100" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockSunnarium", new ItemStack(_SunnariumBlock, 1, 100));</v>
       </c>
       <c r="H100" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_SunnariumBlock);</v>
       </c>
       <c r="K100" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Sunnarium.png</v>
       </c>
       <c r="L100" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Sunnarium = config.get("enabledBlocks", "Sunnarium", true).getBoolean(true);</v>
       </c>
       <c r="N100" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Sunnarium = false;</v>
       </c>
-    </row>
-    <row r="101" spans="1:14">
+      <c r="S100" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockSunnarium.name=Block of Sunnarium</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>105</v>
       </c>
@@ -3950,31 +4356,35 @@
         <v>101</v>
       </c>
       <c r="D101" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _TantalumBlock = new BlockBase("blockTantalum");</v>
       </c>
       <c r="F101" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockTantalum", new ItemStack(_TantalumBlock, 1, 101));</v>
       </c>
       <c r="H101" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_TantalumBlock);</v>
       </c>
       <c r="K101" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Tantalum.png</v>
       </c>
       <c r="L101" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Tantalum = config.get("enabledBlocks", "Tantalum", true).getBoolean(true);</v>
       </c>
       <c r="N101" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Tantalum = false;</v>
       </c>
-    </row>
-    <row r="102" spans="1:14">
+      <c r="S101" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockTantalum.name=Block of Tantalum</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>106</v>
       </c>
@@ -3982,31 +4392,35 @@
         <v>102</v>
       </c>
       <c r="D102" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _TelluriumBlock = new BlockBase("blockTellurium");</v>
       </c>
       <c r="F102" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockTellurium", new ItemStack(_TelluriumBlock, 1, 102));</v>
       </c>
       <c r="H102" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_TelluriumBlock);</v>
       </c>
       <c r="K102" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Tellurium.png</v>
       </c>
       <c r="L102" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Tellurium = config.get("enabledBlocks", "Tellurium", true).getBoolean(true);</v>
       </c>
       <c r="N102" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Tellurium = false;</v>
       </c>
-    </row>
-    <row r="103" spans="1:14">
+      <c r="S102" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockTellurium.name=Block of Tellurium</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>107</v>
       </c>
@@ -4014,31 +4428,35 @@
         <v>103</v>
       </c>
       <c r="D103" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _TerbiumBlock = new BlockBase("blockTerbium");</v>
       </c>
       <c r="F103" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockTerbium", new ItemStack(_TerbiumBlock, 1, 103));</v>
       </c>
       <c r="H103" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_TerbiumBlock);</v>
       </c>
       <c r="K103" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Terbium.png</v>
       </c>
       <c r="L103" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Terbium = config.get("enabledBlocks", "Terbium", true).getBoolean(true);</v>
       </c>
       <c r="N103" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Terbium = false;</v>
       </c>
-    </row>
-    <row r="104" spans="1:14">
+      <c r="S103" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockTerbium.name=Block of Terbium</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>108</v>
       </c>
@@ -4046,31 +4464,35 @@
         <v>104</v>
       </c>
       <c r="D104" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _ThaumiumBlock = new BlockBase("blockThaumium");</v>
       </c>
       <c r="F104" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockThaumium", new ItemStack(_ThaumiumBlock, 1, 104));</v>
       </c>
       <c r="H104" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_ThaumiumBlock);</v>
       </c>
       <c r="K104" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Thaumium.png</v>
       </c>
       <c r="L104" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Thaumium = config.get("enabledBlocks", "Thaumium", true).getBoolean(true);</v>
       </c>
       <c r="N104" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Thaumium = false;</v>
       </c>
-    </row>
-    <row r="105" spans="1:14">
+      <c r="S104" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockThaumium.name=Block of Thaumium</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>109</v>
       </c>
@@ -4078,31 +4500,35 @@
         <v>105</v>
       </c>
       <c r="D105" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _ThoriumBlock = new BlockBase("blockThorium");</v>
       </c>
       <c r="F105" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockThorium", new ItemStack(_ThoriumBlock, 1, 105));</v>
       </c>
       <c r="H105" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_ThoriumBlock);</v>
       </c>
       <c r="K105" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Thorium.png</v>
       </c>
       <c r="L105" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Thorium = config.get("enabledBlocks", "Thorium", true).getBoolean(true);</v>
       </c>
       <c r="N105" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Thorium = false;</v>
       </c>
-    </row>
-    <row r="106" spans="1:14">
+      <c r="S105" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockThorium.name=Block of Thorium</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>110</v>
       </c>
@@ -4110,31 +4536,35 @@
         <v>106</v>
       </c>
       <c r="D106" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _ThuliumBlock = new BlockBase("blockThulium");</v>
       </c>
       <c r="F106" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockThulium", new ItemStack(_ThuliumBlock, 1, 106));</v>
       </c>
       <c r="H106" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_ThuliumBlock);</v>
       </c>
       <c r="K106" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Thulium.png</v>
       </c>
       <c r="L106" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Thulium = config.get("enabledBlocks", "Thulium", true).getBoolean(true);</v>
       </c>
       <c r="N106" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Thulium = false;</v>
       </c>
-    </row>
-    <row r="107" spans="1:14">
+      <c r="S106" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockThulium.name=Block of Thulium</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>111</v>
       </c>
@@ -4142,31 +4572,35 @@
         <v>107</v>
       </c>
       <c r="D107" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _TinAlloyBlock = new BlockBase("blockTinAlloy");</v>
       </c>
       <c r="F107" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockTinAlloy", new ItemStack(_TinAlloyBlock, 1, 107));</v>
       </c>
       <c r="H107" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_TinAlloyBlock);</v>
       </c>
       <c r="K107" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_TinAlloy.png</v>
       </c>
       <c r="L107" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean TinAlloy = config.get("enabledBlocks", "TinAlloy", true).getBoolean(true);</v>
       </c>
       <c r="N107" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean TinAlloy = false;</v>
       </c>
-    </row>
-    <row r="108" spans="1:14">
+      <c r="S107" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockTinAlloy.name=Block of TinAlloy</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>112</v>
       </c>
@@ -4174,31 +4608,35 @@
         <v>108</v>
       </c>
       <c r="D108" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _TinBlock = new BlockBase("blockTin");</v>
       </c>
       <c r="F108" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockTin", new ItemStack(_TinBlock, 1, 108));</v>
       </c>
       <c r="H108" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_TinBlock);</v>
       </c>
       <c r="K108" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Tin.png</v>
       </c>
       <c r="L108" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Tin = config.get("enabledBlocks", "Tin", true).getBoolean(true);</v>
       </c>
       <c r="N108" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Tin = false;</v>
       </c>
-    </row>
-    <row r="109" spans="1:14">
+      <c r="S108" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockTin.name=Block of Tin</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>113</v>
       </c>
@@ -4206,31 +4644,35 @@
         <v>109</v>
       </c>
       <c r="D109" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _TitaniumBlock = new BlockBase("blockTitanium");</v>
       </c>
       <c r="F109" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockTitanium", new ItemStack(_TitaniumBlock, 1, 109));</v>
       </c>
       <c r="H109" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_TitaniumBlock);</v>
       </c>
       <c r="K109" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Titanium.png</v>
       </c>
       <c r="L109" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Titanium = config.get("enabledBlocks", "Titanium", true).getBoolean(true);</v>
       </c>
       <c r="N109" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Titanium = false;</v>
       </c>
-    </row>
-    <row r="110" spans="1:14">
+      <c r="S109" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockTitanium.name=Block of Titanium</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>114</v>
       </c>
@@ -4238,31 +4680,35 @@
         <v>110</v>
       </c>
       <c r="D110" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _TritaniumBlock = new BlockBase("blockTritanium");</v>
       </c>
       <c r="F110" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockTritanium", new ItemStack(_TritaniumBlock, 1, 110));</v>
       </c>
       <c r="H110" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_TritaniumBlock);</v>
       </c>
       <c r="K110" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Tritanium.png</v>
       </c>
       <c r="L110" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Tritanium = config.get("enabledBlocks", "Tritanium", true).getBoolean(true);</v>
       </c>
       <c r="N110" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Tritanium = false;</v>
       </c>
-    </row>
-    <row r="111" spans="1:14">
+      <c r="S110" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockTritanium.name=Block of Tritanium</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>115</v>
       </c>
@@ -4270,31 +4716,35 @@
         <v>111</v>
       </c>
       <c r="D111" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _TungstenSteelBlock = new BlockBase("blockTungstenSteel");</v>
       </c>
       <c r="F111" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockTungstenSteel", new ItemStack(_TungstenSteelBlock, 1, 111));</v>
       </c>
       <c r="H111" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_TungstenSteelBlock);</v>
       </c>
       <c r="K111" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_TungstenSteel.png</v>
       </c>
       <c r="L111" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean TungstenSteel = config.get("enabledBlocks", "TungstenSteel", true).getBoolean(true);</v>
       </c>
       <c r="N111" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean TungstenSteel = false;</v>
       </c>
-    </row>
-    <row r="112" spans="1:14">
+      <c r="S111" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockTungstenSteel.name=Block of TungstenSteel</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>116</v>
       </c>
@@ -4302,31 +4752,35 @@
         <v>112</v>
       </c>
       <c r="D112" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _TungstenBlock = new BlockBase("blockTungsten");</v>
       </c>
       <c r="F112" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockTungsten", new ItemStack(_TungstenBlock, 1, 112));</v>
       </c>
       <c r="H112" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_TungstenBlock);</v>
       </c>
       <c r="K112" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Tungsten.png</v>
       </c>
       <c r="L112" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Tungsten = config.get("enabledBlocks", "Tungsten", true).getBoolean(true);</v>
       </c>
       <c r="N112" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Tungsten = false;</v>
       </c>
-    </row>
-    <row r="113" spans="1:14">
+      <c r="S112" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockTungsten.name=Block of Tungsten</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>117</v>
       </c>
@@ -4334,31 +4788,35 @@
         <v>113</v>
       </c>
       <c r="D113" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _UltimetBlock = new BlockBase("blockUltimet");</v>
       </c>
       <c r="F113" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockUltimet", new ItemStack(_UltimetBlock, 1, 113));</v>
       </c>
       <c r="H113" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_UltimetBlock);</v>
       </c>
       <c r="K113" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Ultimet.png</v>
       </c>
       <c r="L113" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Ultimet = config.get("enabledBlocks", "Ultimet", true).getBoolean(true);</v>
       </c>
       <c r="N113" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Ultimet = false;</v>
       </c>
-    </row>
-    <row r="114" spans="1:14">
+      <c r="S113" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockUltimet.name=Block of Ultimet</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>118</v>
       </c>
@@ -4366,31 +4824,35 @@
         <v>114</v>
       </c>
       <c r="D114" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _Uranium235Block = new BlockBase("blockUranium235");</v>
       </c>
       <c r="F114" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockUranium235", new ItemStack(_Uranium235Block, 1, 114));</v>
       </c>
       <c r="H114" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_Uranium235Block);</v>
       </c>
       <c r="K114" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Uranium235.png</v>
       </c>
       <c r="L114" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Uranium235 = config.get("enabledBlocks", "Uranium235", true).getBoolean(true);</v>
       </c>
       <c r="N114" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Uranium235 = false;</v>
       </c>
-    </row>
-    <row r="115" spans="1:14">
+      <c r="S114" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockUranium235.name=Block of Uranium235</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>119</v>
       </c>
@@ -4398,31 +4860,35 @@
         <v>115</v>
       </c>
       <c r="D115" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _UraniumBlock = new BlockBase("blockUranium");</v>
       </c>
       <c r="F115" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockUranium", new ItemStack(_UraniumBlock, 1, 115));</v>
       </c>
       <c r="H115" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_UraniumBlock);</v>
       </c>
       <c r="K115" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Uranium.png</v>
       </c>
       <c r="L115" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Uranium = config.get("enabledBlocks", "Uranium", true).getBoolean(true);</v>
       </c>
       <c r="N115" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Uranium = false;</v>
       </c>
-    </row>
-    <row r="116" spans="1:14">
+      <c r="S115" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockUranium.name=Block of Uranium</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>120</v>
       </c>
@@ -4430,31 +4896,35 @@
         <v>116</v>
       </c>
       <c r="D116" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _VanadiumGalliumBlock = new BlockBase("blockVanadiumGallium");</v>
       </c>
       <c r="F116" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockVanadiumGallium", new ItemStack(_VanadiumGalliumBlock, 1, 116));</v>
       </c>
       <c r="H116" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_VanadiumGalliumBlock);</v>
       </c>
       <c r="K116" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_VanadiumGallium.png</v>
       </c>
       <c r="L116" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean VanadiumGallium = config.get("enabledBlocks", "VanadiumGallium", true).getBoolean(true);</v>
       </c>
       <c r="N116" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean VanadiumGallium = false;</v>
       </c>
-    </row>
-    <row r="117" spans="1:14">
+      <c r="S116" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockVanadiumGallium.name=Block of VanadiumGallium</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>121</v>
       </c>
@@ -4462,31 +4932,35 @@
         <v>117</v>
       </c>
       <c r="D117" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _VanadiumBlock = new BlockBase("blockVanadium");</v>
       </c>
       <c r="F117" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockVanadium", new ItemStack(_VanadiumBlock, 1, 117));</v>
       </c>
       <c r="H117" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_VanadiumBlock);</v>
       </c>
       <c r="K117" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Vanadium.png</v>
       </c>
       <c r="L117" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Vanadium = config.get("enabledBlocks", "Vanadium", true).getBoolean(true);</v>
       </c>
       <c r="N117" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Vanadium = false;</v>
       </c>
-    </row>
-    <row r="118" spans="1:14">
+      <c r="S117" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockVanadium.name=Block of Vanadium</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>122</v>
       </c>
@@ -4494,31 +4968,35 @@
         <v>118</v>
       </c>
       <c r="D118" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _WroughtIronBlock = new BlockBase("blockWroughtIron");</v>
       </c>
       <c r="F118" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockWroughtIron", new ItemStack(_WroughtIronBlock, 1, 118));</v>
       </c>
       <c r="H118" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_WroughtIronBlock);</v>
       </c>
       <c r="K118" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_WroughtIron.png</v>
       </c>
       <c r="L118" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean WroughtIron = config.get("enabledBlocks", "WroughtIron", true).getBoolean(true);</v>
       </c>
       <c r="N118" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean WroughtIron = false;</v>
       </c>
-    </row>
-    <row r="119" spans="1:14">
+      <c r="S118" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockWroughtIron.name=Block of WroughtIron</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>123</v>
       </c>
@@ -4526,31 +5004,35 @@
         <v>119</v>
       </c>
       <c r="D119" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _YtterbiumBlock = new BlockBase("blockYtterbium");</v>
       </c>
       <c r="F119" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockYtterbium", new ItemStack(_YtterbiumBlock, 1, 119));</v>
       </c>
       <c r="H119" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_YtterbiumBlock);</v>
       </c>
       <c r="K119" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Ytterbium.png</v>
       </c>
       <c r="L119" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Ytterbium = config.get("enabledBlocks", "Ytterbium", true).getBoolean(true);</v>
       </c>
       <c r="N119" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Ytterbium = false;</v>
       </c>
-    </row>
-    <row r="120" spans="1:14">
+      <c r="S119" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockYtterbium.name=Block of Ytterbium</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>124</v>
       </c>
@@ -4558,31 +5040,35 @@
         <v>120</v>
       </c>
       <c r="D120" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _YttriumBariumCuprateBlock = new BlockBase("blockYttriumBariumCuprate");</v>
       </c>
       <c r="F120" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockYttriumBariumCuprate", new ItemStack(_YttriumBariumCuprateBlock, 1, 120));</v>
       </c>
       <c r="H120" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_YttriumBariumCuprateBlock);</v>
       </c>
       <c r="K120" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_YttriumBariumCuprate.png</v>
       </c>
       <c r="L120" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean YttriumBariumCuprate = config.get("enabledBlocks", "YttriumBariumCuprate", true).getBoolean(true);</v>
       </c>
       <c r="N120" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean YttriumBariumCuprate = false;</v>
       </c>
-    </row>
-    <row r="121" spans="1:14">
+      <c r="S120" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockYttriumBariumCuprate.name=Block of YttriumBariumCuprate</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>125</v>
       </c>
@@ -4590,31 +5076,35 @@
         <v>121</v>
       </c>
       <c r="D121" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _YttriumBlock = new BlockBase("blockYttrium");</v>
       </c>
       <c r="F121" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockYttrium", new ItemStack(_YttriumBlock, 1, 121));</v>
       </c>
       <c r="H121" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_YttriumBlock);</v>
       </c>
       <c r="K121" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Yttrium.png</v>
       </c>
       <c r="L121" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Yttrium = config.get("enabledBlocks", "Yttrium", true).getBoolean(true);</v>
       </c>
       <c r="N121" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Yttrium = false;</v>
       </c>
-    </row>
-    <row r="122" spans="1:14">
+      <c r="S121" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockYttrium.name=Block of Yttrium</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>126</v>
       </c>
@@ -4622,31 +5112,35 @@
         <v>122</v>
       </c>
       <c r="D122" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _ZincBlock = new BlockBase("blockZinc");</v>
       </c>
       <c r="F122" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockZinc", new ItemStack(_ZincBlock, 1, 122));</v>
       </c>
       <c r="H122" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_ZincBlock);</v>
       </c>
       <c r="K122" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Zinc.png</v>
       </c>
       <c r="L122" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Zinc = config.get("enabledBlocks", "Zinc", true).getBoolean(true);</v>
       </c>
       <c r="N122" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Zinc = false;</v>
       </c>
-    </row>
-    <row r="123" spans="1:14">
+      <c r="S122" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockZinc.name=Block of Zinc</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>35</v>
       </c>
@@ -4654,31 +5148,35 @@
         <v>123</v>
       </c>
       <c r="D123" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _FieryBloodBlock = new BlockBase("blockFieryBlood");</v>
       </c>
       <c r="F123" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockFieryBlood", new ItemStack(_FieryBloodBlock, 1, 123));</v>
       </c>
       <c r="H123" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_FieryBloodBlock);</v>
       </c>
       <c r="K123" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_FieryBlood.png</v>
       </c>
       <c r="L123" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean FieryBlood = config.get("enabledBlocks", "FieryBlood", true).getBoolean(true);</v>
       </c>
       <c r="N123" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean FieryBlood = false;</v>
       </c>
-    </row>
-    <row r="124" spans="1:14">
+      <c r="S123" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockFieryBlood.name=Block of FieryBlood</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>58</v>
       </c>
@@ -4686,31 +5184,35 @@
         <v>124</v>
       </c>
       <c r="D124" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _MeatRawBlock = new BlockBase("blockMeatRaw");</v>
       </c>
       <c r="F124" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockMeatRaw", new ItemStack(_MeatRawBlock, 1, 124));</v>
       </c>
       <c r="H124" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_MeatRawBlock);</v>
       </c>
       <c r="K124" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_MeatRaw.png</v>
       </c>
       <c r="L124" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean MeatRaw = config.get("enabledBlocks", "MeatRaw", true).getBoolean(true);</v>
       </c>
       <c r="N124" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean MeatRaw = false;</v>
       </c>
-    </row>
-    <row r="125" spans="1:14">
+      <c r="S124" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockMeatRaw.name=Block of MeatRaw</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>80</v>
       </c>
@@ -4718,31 +5220,35 @@
         <v>125</v>
       </c>
       <c r="D125" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _PlasticBlock = new BlockBase("blockPlastic");</v>
       </c>
       <c r="F125" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockPlastic", new ItemStack(_PlasticBlock, 1, 125));</v>
       </c>
       <c r="H125" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_PlasticBlock);</v>
       </c>
       <c r="K125" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Plastic.png</v>
       </c>
       <c r="L125" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Plastic = config.get("enabledBlocks", "Plastic", true).getBoolean(true);</v>
       </c>
       <c r="N125" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Plastic = false;</v>
       </c>
-    </row>
-    <row r="126" spans="1:14">
+      <c r="S125" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockPlastic.name=Block of Plastic</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>89</v>
       </c>
@@ -4750,31 +5256,35 @@
         <v>126</v>
       </c>
       <c r="D126" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _RubberBlock = new BlockBase("blockRubber");</v>
       </c>
       <c r="F126" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockRubber", new ItemStack(_RubberBlock, 1, 126));</v>
       </c>
       <c r="H126" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_RubberBlock);</v>
       </c>
       <c r="K126" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_Rubber.png</v>
       </c>
       <c r="L126" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean Rubber = config.get("enabledBlocks", "Rubber", true).getBoolean(true);</v>
       </c>
       <c r="N126" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean Rubber = false;</v>
       </c>
-    </row>
-    <row r="127" spans="1:14">
+      <c r="S126" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockRubber.name=Block of Rubber</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>99</v>
       </c>
@@ -4782,28 +5292,32 @@
         <v>127</v>
       </c>
       <c r="D127" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>public static Block _SteelLeafBlock = new BlockBase("blockSteelLeaf");</v>
       </c>
       <c r="F127" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>OreDictionary.registerOre("blockSteelLeaf", new ItemStack(_SteelLeafBlock, 1, 127));</v>
       </c>
       <c r="H127" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RegisterHelper.registerBlock(_SteelLeafBlock);</v>
       </c>
       <c r="K127" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>copy dummy.png Block_SteelLeaf.png</v>
       </c>
       <c r="L127" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>public static boolean SteelLeaf = config.get("enabledBlocks", "SteelLeaf", true).getBoolean(true);</v>
       </c>
       <c r="N127" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>public static boolean SteelLeaf = false;</v>
+      </c>
+      <c r="S127" t="str">
+        <f t="shared" si="13"/>
+        <v>tile.blockSteelLeaf.name=Block of SteelLeaf</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prepared loading/saving of block-config
</commit_message>
<xml_diff>
--- a/Mappe1.xlsx
+++ b/Mappe1.xlsx
@@ -715,7 +715,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -723,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K127"/>
+  <dimension ref="A1:N127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E94" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K127"/>
+    <sheetView tabSelected="1" topLeftCell="I100" workbookViewId="0">
+      <selection activeCell="L127" sqref="L127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -735,10 +735,11 @@
     <col min="4" max="4" width="88.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="99.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="109.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -764,8 +765,16 @@
         <f>CONCATENATE("copy dummy.png Block_",A1,".png")</f>
         <v>copy dummy.png Block_Adamantium.png</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" t="str">
+        <f>CONCATENATE("public static boolean ",A1," = config.get(",$B$1,"enabledBlocks",$B$1,", ",$B$1,"",A1,$B$1,", true).getBoolean(true);")</f>
+        <v>public static boolean Adamantium = config.get("enabledBlocks", "Adamantium", true).getBoolean(true);</v>
+      </c>
+      <c r="N1" t="str">
+        <f>CONCATENATE("public static boolean ",A1," = false;")</f>
+        <v>public static boolean Adamantium = false;</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -788,8 +797,16 @@
         <f t="shared" ref="K2:K65" si="3">CONCATENATE("copy dummy.png Block_",A2,".png")</f>
         <v>copy dummy.png Block_Aluminium.png</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:N65" si="4">CONCATENATE("public static boolean ",A2," = config.get(",$B$1,"enabledBlocks",$B$1,", ",$B$1,"",A2,$B$1,", true).getBoolean(true);")</f>
+        <v>public static boolean Aluminium = config.get("enabledBlocks", "Aluminium", true).getBoolean(true);</v>
+      </c>
+      <c r="N2" t="str">
+        <f t="shared" ref="N2:N65" si="5">CONCATENATE("public static boolean ",A2," = false;")</f>
+        <v>public static boolean Aluminium = false;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -812,8 +829,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Americium.png</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Americium = config.get("enabledBlocks", "Americium", true).getBoolean(true);</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Americium = false;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -836,8 +861,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_AnnealedCopper.png</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean AnnealedCopper = config.get("enabledBlocks", "AnnealedCopper", true).getBoolean(true);</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean AnnealedCopper = false;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -860,8 +893,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Antimony.png</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Antimony = config.get("enabledBlocks", "Antimony", true).getBoolean(true);</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Antimony = false;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -884,8 +925,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_AstralSilver.png</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean AstralSilver = config.get("enabledBlocks", "AstralSilver", true).getBoolean(true);</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean AstralSilver = false;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -908,8 +957,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_BatteryAlloy.png</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean BatteryAlloy = config.get("enabledBlocks", "BatteryAlloy", true).getBoolean(true);</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean BatteryAlloy = false;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -932,8 +989,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Beryllium.png</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Beryllium = config.get("enabledBlocks", "Beryllium", true).getBoolean(true);</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Beryllium = false;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -956,8 +1021,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_BismuthBronze.png</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean BismuthBronze = config.get("enabledBlocks", "BismuthBronze", true).getBoolean(true);</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean BismuthBronze = false;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -980,8 +1053,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Bismuth.png</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Bismuth = config.get("enabledBlocks", "Bismuth", true).getBoolean(true);</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Bismuth = false;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1004,8 +1085,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_BlackBronze.png</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean BlackBronze = config.get("enabledBlocks", "BlackBronze", true).getBoolean(true);</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean BlackBronze = false;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1028,8 +1117,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_BlackSteel.png</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean BlackSteel = config.get("enabledBlocks", "BlackSteel", true).getBoolean(true);</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean BlackSteel = false;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1052,8 +1149,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_BlueAlloy.png</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean BlueAlloy = config.get("enabledBlocks", "BlueAlloy", true).getBoolean(true);</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean BlueAlloy = false;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1076,8 +1181,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_BlueSteel.png</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean BlueSteel = config.get("enabledBlocks", "BlueSteel", true).getBoolean(true);</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean BlueSteel = false;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1100,8 +1213,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Brass.png</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Brass = config.get("enabledBlocks", "Brass", true).getBoolean(true);</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Brass = false;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1124,8 +1245,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Bronze.png</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Bronze = config.get("enabledBlocks", "Bronze", true).getBoolean(true);</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Bronze = false;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1148,8 +1277,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Caesium.png</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Caesium = config.get("enabledBlocks", "Caesium", true).getBoolean(true);</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Caesium = false;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1172,8 +1309,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Cerium.png</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Cerium = config.get("enabledBlocks", "Cerium", true).getBoolean(true);</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Cerium = false;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1196,8 +1341,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Chrome.png</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Chrome = config.get("enabledBlocks", "Chrome", true).getBoolean(true);</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Chrome = false;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1220,8 +1373,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_ChromiumDioxide.png</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean ChromiumDioxide = config.get("enabledBlocks", "ChromiumDioxide", true).getBoolean(true);</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean ChromiumDioxide = false;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1244,8 +1405,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_CobaltBrass.png</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="L21" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean CobaltBrass = config.get("enabledBlocks", "CobaltBrass", true).getBoolean(true);</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean CobaltBrass = false;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1268,8 +1437,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Cobalt.png</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Cobalt = config.get("enabledBlocks", "Cobalt", true).getBoolean(true);</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Cobalt = false;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1292,8 +1469,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Copper.png</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="L23" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Copper = config.get("enabledBlocks", "Copper", true).getBoolean(true);</v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Copper = false;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1316,8 +1501,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Cupronickel.png</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="L24" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Cupronickel = config.get("enabledBlocks", "Cupronickel", true).getBoolean(true);</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Cupronickel = false;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1340,8 +1533,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_DamascusSteel.png</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="L25" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean DamascusSteel = config.get("enabledBlocks", "DamascusSteel", true).getBoolean(true);</v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean DamascusSteel = false;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1364,8 +1565,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_DarkIron.png</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="L26" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean DarkIron = config.get("enabledBlocks", "DarkIron", true).getBoolean(true);</v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean DarkIron = false;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1388,8 +1597,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_DeepIron.png</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="L27" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean DeepIron = config.get("enabledBlocks", "DeepIron", true).getBoolean(true);</v>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean DeepIron = false;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1412,8 +1629,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Desh.png</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="L28" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Desh = config.get("enabledBlocks", "Desh", true).getBoolean(true);</v>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Desh = false;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1436,8 +1661,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Duranium.png</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="L29" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Duranium = config.get("enabledBlocks", "Duranium", true).getBoolean(true);</v>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Duranium = false;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1460,8 +1693,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Dysprosium.png</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="L30" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Dysprosium = config.get("enabledBlocks", "Dysprosium", true).getBoolean(true);</v>
+      </c>
+      <c r="N30" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Dysprosium = false;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1484,8 +1725,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_ElectrumFlux.png</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="L31" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean ElectrumFlux = config.get("enabledBlocks", "ElectrumFlux", true).getBoolean(true);</v>
+      </c>
+      <c r="N31" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean ElectrumFlux = false;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1508,8 +1757,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Electrum.png</v>
       </c>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="L32" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Electrum = config.get("enabledBlocks", "Electrum", true).getBoolean(true);</v>
+      </c>
+      <c r="N32" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Electrum = false;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1532,8 +1789,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Enderium.png</v>
       </c>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="L33" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Enderium = config.get("enabledBlocks", "Enderium", true).getBoolean(true);</v>
+      </c>
+      <c r="N33" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Enderium = false;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1556,8 +1821,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Erbium.png</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="L34" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Erbium = config.get("enabledBlocks", "Erbium", true).getBoolean(true);</v>
+      </c>
+      <c r="N34" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Erbium = false;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1580,8 +1853,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Europium.png</v>
       </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="L35" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Europium = config.get("enabledBlocks", "Europium", true).getBoolean(true);</v>
+      </c>
+      <c r="N35" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Europium = false;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1604,8 +1885,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_FierySteel.png</v>
       </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="L36" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean FierySteel = config.get("enabledBlocks", "FierySteel", true).getBoolean(true);</v>
+      </c>
+      <c r="N36" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean FierySteel = false;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1628,8 +1917,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Force.png</v>
       </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="L37" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Force = config.get("enabledBlocks", "Force", true).getBoolean(true);</v>
+      </c>
+      <c r="N37" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Force = false;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1652,8 +1949,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Gadolinium.png</v>
       </c>
-    </row>
-    <row r="39" spans="1:11">
+      <c r="L38" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Gadolinium = config.get("enabledBlocks", "Gadolinium", true).getBoolean(true);</v>
+      </c>
+      <c r="N38" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Gadolinium = false;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1676,8 +1981,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Gallium.png</v>
       </c>
-    </row>
-    <row r="40" spans="1:11">
+      <c r="L39" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Gallium = config.get("enabledBlocks", "Gallium", true).getBoolean(true);</v>
+      </c>
+      <c r="N39" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Gallium = false;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1700,8 +2013,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Gold.png</v>
       </c>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="L40" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Gold = config.get("enabledBlocks", "Gold", true).getBoolean(true);</v>
+      </c>
+      <c r="N40" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Gold = false;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1724,8 +2045,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_HSLA.png</v>
       </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="L41" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean HSLA = config.get("enabledBlocks", "HSLA", true).getBoolean(true);</v>
+      </c>
+      <c r="N41" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean HSLA = false;</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1748,8 +2077,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Holmium.png</v>
       </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="L42" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Holmium = config.get("enabledBlocks", "Holmium", true).getBoolean(true);</v>
+      </c>
+      <c r="N42" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Holmium = false;</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1772,8 +2109,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Indium.png</v>
       </c>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="L43" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Indium = config.get("enabledBlocks", "Indium", true).getBoolean(true);</v>
+      </c>
+      <c r="N43" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Indium = false;</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1796,8 +2141,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_InfusedGold.png</v>
       </c>
-    </row>
-    <row r="45" spans="1:11">
+      <c r="L44" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean InfusedGold = config.get("enabledBlocks", "InfusedGold", true).getBoolean(true);</v>
+      </c>
+      <c r="N44" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean InfusedGold = false;</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -1820,8 +2173,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Invar.png</v>
       </c>
-    </row>
-    <row r="46" spans="1:11">
+      <c r="L45" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Invar = config.get("enabledBlocks", "Invar", true).getBoolean(true);</v>
+      </c>
+      <c r="N45" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Invar = false;</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1844,8 +2205,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Iridium.png</v>
       </c>
-    </row>
-    <row r="47" spans="1:11">
+      <c r="L46" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Iridium = config.get("enabledBlocks", "Iridium", true).getBoolean(true);</v>
+      </c>
+      <c r="N46" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Iridium = false;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1868,8 +2237,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_IronMagnetic.png</v>
       </c>
-    </row>
-    <row r="48" spans="1:11">
+      <c r="L47" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean IronMagnetic = config.get("enabledBlocks", "IronMagnetic", true).getBoolean(true);</v>
+      </c>
+      <c r="N47" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean IronMagnetic = false;</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1892,8 +2269,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_IronWood.png</v>
       </c>
-    </row>
-    <row r="49" spans="1:11">
+      <c r="L48" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean IronWood = config.get("enabledBlocks", "IronWood", true).getBoolean(true);</v>
+      </c>
+      <c r="N48" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean IronWood = false;</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1916,8 +2301,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Iron.png</v>
       </c>
-    </row>
-    <row r="50" spans="1:11">
+      <c r="L49" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Iron = config.get("enabledBlocks", "Iron", true).getBoolean(true);</v>
+      </c>
+      <c r="N49" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Iron = false;</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -1940,8 +2333,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Kanthal.png</v>
       </c>
-    </row>
-    <row r="51" spans="1:11">
+      <c r="L50" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Kanthal = config.get("enabledBlocks", "Kanthal", true).getBoolean(true);</v>
+      </c>
+      <c r="N50" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Kanthal = false;</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -1964,8 +2365,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Knightmetal.png</v>
       </c>
-    </row>
-    <row r="52" spans="1:11">
+      <c r="L51" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Knightmetal = config.get("enabledBlocks", "Knightmetal", true).getBoolean(true);</v>
+      </c>
+      <c r="N51" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Knightmetal = false;</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1988,8 +2397,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Lanthanum.png</v>
       </c>
-    </row>
-    <row r="53" spans="1:11">
+      <c r="L52" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Lanthanum = config.get("enabledBlocks", "Lanthanum", true).getBoolean(true);</v>
+      </c>
+      <c r="N52" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Lanthanum = false;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2012,8 +2429,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Lead.png</v>
       </c>
-    </row>
-    <row r="54" spans="1:11">
+      <c r="L53" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Lead = config.get("enabledBlocks", "Lead", true).getBoolean(true);</v>
+      </c>
+      <c r="N53" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Lead = false;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2036,8 +2461,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Lutetium.png</v>
       </c>
-    </row>
-    <row r="55" spans="1:11">
+      <c r="L54" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Lutetium = config.get("enabledBlocks", "Lutetium", true).getBoolean(true);</v>
+      </c>
+      <c r="N54" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Lutetium = false;</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2060,8 +2493,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Magnalium.png</v>
       </c>
-    </row>
-    <row r="56" spans="1:11">
+      <c r="L55" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Magnalium = config.get("enabledBlocks", "Magnalium", true).getBoolean(true);</v>
+      </c>
+      <c r="N55" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Magnalium = false;</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2084,8 +2525,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Magnesium.png</v>
       </c>
-    </row>
-    <row r="57" spans="1:11">
+      <c r="L56" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Magnesium = config.get("enabledBlocks", "Magnesium", true).getBoolean(true);</v>
+      </c>
+      <c r="N56" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Magnesium = false;</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -2108,8 +2557,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Manganese.png</v>
       </c>
-    </row>
-    <row r="58" spans="1:11">
+      <c r="L57" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Manganese = config.get("enabledBlocks", "Manganese", true).getBoolean(true);</v>
+      </c>
+      <c r="N57" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Manganese = false;</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -2132,8 +2589,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_MeteoricIron.png</v>
       </c>
-    </row>
-    <row r="59" spans="1:11">
+      <c r="L58" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean MeteoricIron = config.get("enabledBlocks", "MeteoricIron", true).getBoolean(true);</v>
+      </c>
+      <c r="N58" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean MeteoricIron = false;</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -2156,8 +2621,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_MeteoricSteel.png</v>
       </c>
-    </row>
-    <row r="60" spans="1:11">
+      <c r="L59" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean MeteoricSteel = config.get("enabledBlocks", "MeteoricSteel", true).getBoolean(true);</v>
+      </c>
+      <c r="N59" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean MeteoricSteel = false;</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -2180,8 +2653,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Midasium.png</v>
       </c>
-    </row>
-    <row r="61" spans="1:11">
+      <c r="L60" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Midasium = config.get("enabledBlocks", "Midasium", true).getBoolean(true);</v>
+      </c>
+      <c r="N60" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Midasium = false;</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
       <c r="A61" t="s">
         <v>62</v>
       </c>
@@ -2204,8 +2685,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Mithril.png</v>
       </c>
-    </row>
-    <row r="62" spans="1:11">
+      <c r="L61" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Mithril = config.get("enabledBlocks", "Mithril", true).getBoolean(true);</v>
+      </c>
+      <c r="N61" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Mithril = false;</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -2228,8 +2717,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Molybdenum.png</v>
       </c>
-    </row>
-    <row r="63" spans="1:11">
+      <c r="L62" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Molybdenum = config.get("enabledBlocks", "Molybdenum", true).getBoolean(true);</v>
+      </c>
+      <c r="N62" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Molybdenum = false;</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -2252,8 +2749,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_NaquadahAlloy.png</v>
       </c>
-    </row>
-    <row r="64" spans="1:11">
+      <c r="L63" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean NaquadahAlloy = config.get("enabledBlocks", "NaquadahAlloy", true).getBoolean(true);</v>
+      </c>
+      <c r="N63" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean NaquadahAlloy = false;</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -2276,8 +2781,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_NaquadahEnriched.png</v>
       </c>
-    </row>
-    <row r="65" spans="1:11">
+      <c r="L64" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean NaquadahEnriched = config.get("enabledBlocks", "NaquadahEnriched", true).getBoolean(true);</v>
+      </c>
+      <c r="N64" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean NaquadahEnriched = false;</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -2300,8 +2813,16 @@
         <f t="shared" si="3"/>
         <v>copy dummy.png Block_Naquadah.png</v>
       </c>
-    </row>
-    <row r="66" spans="1:11">
+      <c r="L65" t="str">
+        <f t="shared" si="4"/>
+        <v>public static boolean Naquadah = config.get("enabledBlocks", "Naquadah", true).getBoolean(true);</v>
+      </c>
+      <c r="N65" t="str">
+        <f t="shared" si="5"/>
+        <v>public static boolean Naquadah = false;</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -2309,23 +2830,31 @@
         <v>66</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" ref="D66:D127" si="4">CONCATENATE("public static Block _",A66,"Block = new BlockBase(",$B$1,"block",A66,$B$1,");")</f>
+        <f t="shared" ref="D66:D127" si="6">CONCATENATE("public static Block _",A66,"Block = new BlockBase(",$B$1,"block",A66,$B$1,");")</f>
         <v>public static Block _NaquadriaBlock = new BlockBase("blockNaquadria");</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" ref="F66:F127" si="5">CONCATENATE("OreDictionary.registerOre(",$B$1,"block",A66,$B$1,", new ItemStack(_",A66,"Block, 1, ",C66,"));")</f>
+        <f t="shared" ref="F66:F127" si="7">CONCATENATE("OreDictionary.registerOre(",$B$1,"block",A66,$B$1,", new ItemStack(_",A66,"Block, 1, ",C66,"));")</f>
         <v>OreDictionary.registerOre("blockNaquadria", new ItemStack(_NaquadriaBlock, 1, 66));</v>
       </c>
       <c r="H66" t="str">
-        <f t="shared" ref="H66:H127" si="6">CONCATENATE("RegisterHelper.registerBlock(_",A66,"Block);")</f>
+        <f t="shared" ref="H66:H127" si="8">CONCATENATE("RegisterHelper.registerBlock(_",A66,"Block);")</f>
         <v>RegisterHelper.registerBlock(_NaquadriaBlock);</v>
       </c>
       <c r="K66" t="str">
-        <f t="shared" ref="K66:K127" si="7">CONCATENATE("copy dummy.png Block_",A66,".png")</f>
+        <f t="shared" ref="K66:K127" si="9">CONCATENATE("copy dummy.png Block_",A66,".png")</f>
         <v>copy dummy.png Block_Naquadria.png</v>
       </c>
-    </row>
-    <row r="67" spans="1:11">
+      <c r="L66" t="str">
+        <f t="shared" ref="L66:N127" si="10">CONCATENATE("public static boolean ",A66," = config.get(",$B$1,"enabledBlocks",$B$1,", ",$B$1,"",A66,$B$1,", true).getBoolean(true);")</f>
+        <v>public static boolean Naquadria = config.get("enabledBlocks", "Naquadria", true).getBoolean(true);</v>
+      </c>
+      <c r="N66" t="str">
+        <f t="shared" ref="N66:N127" si="11">CONCATENATE("public static boolean ",A66," = false;")</f>
+        <v>public static boolean Naquadria = false;</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
       <c r="A67" t="s">
         <v>68</v>
       </c>
@@ -2333,23 +2862,31 @@
         <v>67</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _NeodymiumMagneticBlock = new BlockBase("blockNeodymiumMagnetic");</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockNeodymiumMagnetic", new ItemStack(_NeodymiumMagneticBlock, 1, 67));</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_NeodymiumMagneticBlock);</v>
       </c>
       <c r="K67" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_NeodymiumMagnetic.png</v>
       </c>
-    </row>
-    <row r="68" spans="1:11">
+      <c r="L67" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean NeodymiumMagnetic = config.get("enabledBlocks", "NeodymiumMagnetic", true).getBoolean(true);</v>
+      </c>
+      <c r="N67" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean NeodymiumMagnetic = false;</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
       <c r="A68" t="s">
         <v>69</v>
       </c>
@@ -2357,23 +2894,31 @@
         <v>68</v>
       </c>
       <c r="D68" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _NeodymiumBlock = new BlockBase("blockNeodymium");</v>
       </c>
       <c r="F68" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockNeodymium", new ItemStack(_NeodymiumBlock, 1, 68));</v>
       </c>
       <c r="H68" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_NeodymiumBlock);</v>
       </c>
       <c r="K68" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Neodymium.png</v>
       </c>
-    </row>
-    <row r="69" spans="1:11">
+      <c r="L68" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Neodymium = config.get("enabledBlocks", "Neodymium", true).getBoolean(true);</v>
+      </c>
+      <c r="N68" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Neodymium = false;</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -2381,23 +2926,31 @@
         <v>69</v>
       </c>
       <c r="D69" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _NeutroniumBlock = new BlockBase("blockNeutronium");</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockNeutronium", new ItemStack(_NeutroniumBlock, 1, 69));</v>
       </c>
       <c r="H69" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_NeutroniumBlock);</v>
       </c>
       <c r="K69" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Neutronium.png</v>
       </c>
-    </row>
-    <row r="70" spans="1:11">
+      <c r="L69" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Neutronium = config.get("enabledBlocks", "Neutronium", true).getBoolean(true);</v>
+      </c>
+      <c r="N69" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Neutronium = false;</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14">
       <c r="A70" t="s">
         <v>71</v>
       </c>
@@ -2405,23 +2958,31 @@
         <v>70</v>
       </c>
       <c r="D70" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _NichromeBlock = new BlockBase("blockNichrome");</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockNichrome", new ItemStack(_NichromeBlock, 1, 70));</v>
       </c>
       <c r="H70" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_NichromeBlock);</v>
       </c>
       <c r="K70" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Nichrome.png</v>
       </c>
-    </row>
-    <row r="71" spans="1:11">
+      <c r="L70" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Nichrome = config.get("enabledBlocks", "Nichrome", true).getBoolean(true);</v>
+      </c>
+      <c r="N70" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Nichrome = false;</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14">
       <c r="A71" t="s">
         <v>72</v>
       </c>
@@ -2429,23 +2990,31 @@
         <v>71</v>
       </c>
       <c r="D71" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _NickelBlock = new BlockBase("blockNickel");</v>
       </c>
       <c r="F71" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockNickel", new ItemStack(_NickelBlock, 1, 71));</v>
       </c>
       <c r="H71" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_NickelBlock);</v>
       </c>
       <c r="K71" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Nickel.png</v>
       </c>
-    </row>
-    <row r="72" spans="1:11">
+      <c r="L71" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Nickel = config.get("enabledBlocks", "Nickel", true).getBoolean(true);</v>
+      </c>
+      <c r="N71" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Nickel = false;</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14">
       <c r="A72" t="s">
         <v>73</v>
       </c>
@@ -2453,23 +3022,31 @@
         <v>72</v>
       </c>
       <c r="D72" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _NiobiumNitrideBlock = new BlockBase("blockNiobiumNitride");</v>
       </c>
       <c r="F72" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockNiobiumNitride", new ItemStack(_NiobiumNitrideBlock, 1, 72));</v>
       </c>
       <c r="H72" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_NiobiumNitrideBlock);</v>
       </c>
       <c r="K72" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_NiobiumNitride.png</v>
       </c>
-    </row>
-    <row r="73" spans="1:11">
+      <c r="L72" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean NiobiumNitride = config.get("enabledBlocks", "NiobiumNitride", true).getBoolean(true);</v>
+      </c>
+      <c r="N72" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean NiobiumNitride = false;</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14">
       <c r="A73" t="s">
         <v>74</v>
       </c>
@@ -2477,23 +3054,31 @@
         <v>73</v>
       </c>
       <c r="D73" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _NiobiumTitaniumBlock = new BlockBase("blockNiobiumTitanium");</v>
       </c>
       <c r="F73" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockNiobiumTitanium", new ItemStack(_NiobiumTitaniumBlock, 1, 73));</v>
       </c>
       <c r="H73" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_NiobiumTitaniumBlock);</v>
       </c>
       <c r="K73" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_NiobiumTitanium.png</v>
       </c>
-    </row>
-    <row r="74" spans="1:11">
+      <c r="L73" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean NiobiumTitanium = config.get("enabledBlocks", "NiobiumTitanium", true).getBoolean(true);</v>
+      </c>
+      <c r="N73" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean NiobiumTitanium = false;</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14">
       <c r="A74" t="s">
         <v>75</v>
       </c>
@@ -2501,23 +3086,31 @@
         <v>74</v>
       </c>
       <c r="D74" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _NiobiumBlock = new BlockBase("blockNiobium");</v>
       </c>
       <c r="F74" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockNiobium", new ItemStack(_NiobiumBlock, 1, 74));</v>
       </c>
       <c r="H74" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_NiobiumBlock);</v>
       </c>
       <c r="K74" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Niobium.png</v>
       </c>
-    </row>
-    <row r="75" spans="1:11">
+      <c r="L74" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Niobium = config.get("enabledBlocks", "Niobium", true).getBoolean(true);</v>
+      </c>
+      <c r="N74" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Niobium = false;</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14">
       <c r="A75" t="s">
         <v>76</v>
       </c>
@@ -2525,23 +3118,31 @@
         <v>75</v>
       </c>
       <c r="D75" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _OsmiridiumBlock = new BlockBase("blockOsmiridium");</v>
       </c>
       <c r="F75" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockOsmiridium", new ItemStack(_OsmiridiumBlock, 1, 75));</v>
       </c>
       <c r="H75" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_OsmiridiumBlock);</v>
       </c>
       <c r="K75" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Osmiridium.png</v>
       </c>
-    </row>
-    <row r="76" spans="1:11">
+      <c r="L75" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Osmiridium = config.get("enabledBlocks", "Osmiridium", true).getBoolean(true);</v>
+      </c>
+      <c r="N75" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Osmiridium = false;</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14">
       <c r="A76" t="s">
         <v>77</v>
       </c>
@@ -2549,23 +3150,31 @@
         <v>76</v>
       </c>
       <c r="D76" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _OsmiumBlock = new BlockBase("blockOsmium");</v>
       </c>
       <c r="F76" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockOsmium", new ItemStack(_OsmiumBlock, 1, 76));</v>
       </c>
       <c r="H76" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_OsmiumBlock);</v>
       </c>
       <c r="K76" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Osmium.png</v>
       </c>
-    </row>
-    <row r="77" spans="1:11">
+      <c r="L76" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Osmium = config.get("enabledBlocks", "Osmium", true).getBoolean(true);</v>
+      </c>
+      <c r="N76" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Osmium = false;</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14">
       <c r="A77" t="s">
         <v>78</v>
       </c>
@@ -2573,23 +3182,31 @@
         <v>77</v>
       </c>
       <c r="D77" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _PalladiumBlock = new BlockBase("blockPalladium");</v>
       </c>
       <c r="F77" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockPalladium", new ItemStack(_PalladiumBlock, 1, 77));</v>
       </c>
       <c r="H77" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_PalladiumBlock);</v>
       </c>
       <c r="K77" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Palladium.png</v>
       </c>
-    </row>
-    <row r="78" spans="1:11">
+      <c r="L77" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Palladium = config.get("enabledBlocks", "Palladium", true).getBoolean(true);</v>
+      </c>
+      <c r="N77" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Palladium = false;</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14">
       <c r="A78" t="s">
         <v>79</v>
       </c>
@@ -2597,23 +3214,31 @@
         <v>78</v>
       </c>
       <c r="D78" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _PigIronBlock = new BlockBase("blockPigIron");</v>
       </c>
       <c r="F78" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockPigIron", new ItemStack(_PigIronBlock, 1, 78));</v>
       </c>
       <c r="H78" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_PigIronBlock);</v>
       </c>
       <c r="K78" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_PigIron.png</v>
       </c>
-    </row>
-    <row r="79" spans="1:11">
+      <c r="L78" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean PigIron = config.get("enabledBlocks", "PigIron", true).getBoolean(true);</v>
+      </c>
+      <c r="N78" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean PigIron = false;</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14">
       <c r="A79" t="s">
         <v>81</v>
       </c>
@@ -2621,23 +3246,31 @@
         <v>79</v>
       </c>
       <c r="D79" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _PlatinumBlock = new BlockBase("blockPlatinum");</v>
       </c>
       <c r="F79" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockPlatinum", new ItemStack(_PlatinumBlock, 1, 79));</v>
       </c>
       <c r="H79" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_PlatinumBlock);</v>
       </c>
       <c r="K79" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Platinum.png</v>
       </c>
-    </row>
-    <row r="80" spans="1:11">
+      <c r="L79" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Platinum = config.get("enabledBlocks", "Platinum", true).getBoolean(true);</v>
+      </c>
+      <c r="N79" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Platinum = false;</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -2645,23 +3278,31 @@
         <v>80</v>
       </c>
       <c r="D80" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _Plutonium241Block = new BlockBase("blockPlutonium241");</v>
       </c>
       <c r="F80" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockPlutonium241", new ItemStack(_Plutonium241Block, 1, 80));</v>
       </c>
       <c r="H80" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_Plutonium241Block);</v>
       </c>
       <c r="K80" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Plutonium241.png</v>
       </c>
-    </row>
-    <row r="81" spans="1:11">
+      <c r="L80" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Plutonium241 = config.get("enabledBlocks", "Plutonium241", true).getBoolean(true);</v>
+      </c>
+      <c r="N80" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Plutonium241 = false;</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14">
       <c r="A81" t="s">
         <v>83</v>
       </c>
@@ -2669,23 +3310,31 @@
         <v>81</v>
       </c>
       <c r="D81" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _PlutoniumBlock = new BlockBase("blockPlutonium");</v>
       </c>
       <c r="F81" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockPlutonium", new ItemStack(_PlutoniumBlock, 1, 81));</v>
       </c>
       <c r="H81" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_PlutoniumBlock);</v>
       </c>
       <c r="K81" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Plutonium.png</v>
       </c>
-    </row>
-    <row r="82" spans="1:11">
+      <c r="L81" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Plutonium = config.get("enabledBlocks", "Plutonium", true).getBoolean(true);</v>
+      </c>
+      <c r="N81" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Plutonium = false;</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14">
       <c r="A82" t="s">
         <v>84</v>
       </c>
@@ -2693,23 +3342,31 @@
         <v>82</v>
       </c>
       <c r="D82" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _PraseodymiumBlock = new BlockBase("blockPraseodymium");</v>
       </c>
       <c r="F82" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockPraseodymium", new ItemStack(_PraseodymiumBlock, 1, 82));</v>
       </c>
       <c r="H82" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_PraseodymiumBlock);</v>
       </c>
       <c r="K82" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Praseodymium.png</v>
       </c>
-    </row>
-    <row r="83" spans="1:11">
+      <c r="L82" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Praseodymium = config.get("enabledBlocks", "Praseodymium", true).getBoolean(true);</v>
+      </c>
+      <c r="N82" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Praseodymium = false;</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14">
       <c r="A83" t="s">
         <v>85</v>
       </c>
@@ -2717,23 +3374,31 @@
         <v>83</v>
       </c>
       <c r="D83" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _PromethiumBlock = new BlockBase("blockPromethium");</v>
       </c>
       <c r="F83" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockPromethium", new ItemStack(_PromethiumBlock, 1, 83));</v>
       </c>
       <c r="H83" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_PromethiumBlock);</v>
       </c>
       <c r="K83" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Promethium.png</v>
       </c>
-    </row>
-    <row r="84" spans="1:11">
+      <c r="L83" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Promethium = config.get("enabledBlocks", "Promethium", true).getBoolean(true);</v>
+      </c>
+      <c r="N83" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Promethium = false;</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14">
       <c r="A84" t="s">
         <v>86</v>
       </c>
@@ -2741,23 +3406,31 @@
         <v>84</v>
       </c>
       <c r="D84" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _RedAlloyBlock = new BlockBase("blockRedAlloy");</v>
       </c>
       <c r="F84" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockRedAlloy", new ItemStack(_RedAlloyBlock, 1, 84));</v>
       </c>
       <c r="H84" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_RedAlloyBlock);</v>
       </c>
       <c r="K84" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_RedAlloy.png</v>
       </c>
-    </row>
-    <row r="85" spans="1:11">
+      <c r="L84" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean RedAlloy = config.get("enabledBlocks", "RedAlloy", true).getBoolean(true);</v>
+      </c>
+      <c r="N84" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean RedAlloy = false;</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14">
       <c r="A85" t="s">
         <v>87</v>
       </c>
@@ -2765,23 +3438,31 @@
         <v>85</v>
       </c>
       <c r="D85" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _RedSteelBlock = new BlockBase("blockRedSteel");</v>
       </c>
       <c r="F85" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockRedSteel", new ItemStack(_RedSteelBlock, 1, 85));</v>
       </c>
       <c r="H85" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_RedSteelBlock);</v>
       </c>
       <c r="K85" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_RedSteel.png</v>
       </c>
-    </row>
-    <row r="86" spans="1:11">
+      <c r="L85" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean RedSteel = config.get("enabledBlocks", "RedSteel", true).getBoolean(true);</v>
+      </c>
+      <c r="N85" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean RedSteel = false;</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14">
       <c r="A86" t="s">
         <v>88</v>
       </c>
@@ -2789,23 +3470,31 @@
         <v>86</v>
       </c>
       <c r="D86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _RoseGoldBlock = new BlockBase("blockRoseGold");</v>
       </c>
       <c r="F86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockRoseGold", new ItemStack(_RoseGoldBlock, 1, 86));</v>
       </c>
       <c r="H86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_RoseGoldBlock);</v>
       </c>
       <c r="K86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_RoseGold.png</v>
       </c>
-    </row>
-    <row r="87" spans="1:11">
+      <c r="L86" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean RoseGold = config.get("enabledBlocks", "RoseGold", true).getBoolean(true);</v>
+      </c>
+      <c r="N86" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean RoseGold = false;</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14">
       <c r="A87" t="s">
         <v>90</v>
       </c>
@@ -2813,23 +3502,31 @@
         <v>87</v>
       </c>
       <c r="D87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _RubidiumBlock = new BlockBase("blockRubidium");</v>
       </c>
       <c r="F87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockRubidium", new ItemStack(_RubidiumBlock, 1, 87));</v>
       </c>
       <c r="H87" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_RubidiumBlock);</v>
       </c>
       <c r="K87" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Rubidium.png</v>
       </c>
-    </row>
-    <row r="88" spans="1:11">
+      <c r="L87" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Rubidium = config.get("enabledBlocks", "Rubidium", true).getBoolean(true);</v>
+      </c>
+      <c r="N87" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Rubidium = false;</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14">
       <c r="A88" t="s">
         <v>91</v>
       </c>
@@ -2837,23 +3534,31 @@
         <v>88</v>
       </c>
       <c r="D88" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _SamariumBlock = new BlockBase("blockSamarium");</v>
       </c>
       <c r="F88" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockSamarium", new ItemStack(_SamariumBlock, 1, 88));</v>
       </c>
       <c r="H88" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_SamariumBlock);</v>
       </c>
       <c r="K88" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Samarium.png</v>
       </c>
-    </row>
-    <row r="89" spans="1:11">
+      <c r="L88" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Samarium = config.get("enabledBlocks", "Samarium", true).getBoolean(true);</v>
+      </c>
+      <c r="N88" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Samarium = false;</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14">
       <c r="A89" t="s">
         <v>92</v>
       </c>
@@ -2861,23 +3566,31 @@
         <v>89</v>
       </c>
       <c r="D89" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _ScandiumBlock = new BlockBase("blockScandium");</v>
       </c>
       <c r="F89" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockScandium", new ItemStack(_ScandiumBlock, 1, 89));</v>
       </c>
       <c r="H89" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_ScandiumBlock);</v>
       </c>
       <c r="K89" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Scandium.png</v>
       </c>
-    </row>
-    <row r="90" spans="1:11">
+      <c r="L89" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Scandium = config.get("enabledBlocks", "Scandium", true).getBoolean(true);</v>
+      </c>
+      <c r="N89" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Scandium = false;</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14">
       <c r="A90" t="s">
         <v>93</v>
       </c>
@@ -2885,23 +3598,31 @@
         <v>90</v>
       </c>
       <c r="D90" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _ShadowIronBlock = new BlockBase("blockShadowIron");</v>
       </c>
       <c r="F90" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockShadowIron", new ItemStack(_ShadowIronBlock, 1, 90));</v>
       </c>
       <c r="H90" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_ShadowIronBlock);</v>
       </c>
       <c r="K90" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_ShadowIron.png</v>
       </c>
-    </row>
-    <row r="91" spans="1:11">
+      <c r="L90" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean ShadowIron = config.get("enabledBlocks", "ShadowIron", true).getBoolean(true);</v>
+      </c>
+      <c r="N90" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean ShadowIron = false;</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14">
       <c r="A91" t="s">
         <v>94</v>
       </c>
@@ -2909,23 +3630,31 @@
         <v>91</v>
       </c>
       <c r="D91" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _ShadowSteelBlock = new BlockBase("blockShadowSteel");</v>
       </c>
       <c r="F91" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockShadowSteel", new ItemStack(_ShadowSteelBlock, 1, 91));</v>
       </c>
       <c r="H91" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_ShadowSteelBlock);</v>
       </c>
       <c r="K91" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_ShadowSteel.png</v>
       </c>
-    </row>
-    <row r="92" spans="1:11">
+      <c r="L91" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean ShadowSteel = config.get("enabledBlocks", "ShadowSteel", true).getBoolean(true);</v>
+      </c>
+      <c r="N91" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean ShadowSteel = false;</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -2933,23 +3662,31 @@
         <v>92</v>
       </c>
       <c r="D92" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _SiliconBlock = new BlockBase("blockSilicon");</v>
       </c>
       <c r="F92" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockSilicon", new ItemStack(_SiliconBlock, 1, 92));</v>
       </c>
       <c r="H92" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_SiliconBlock);</v>
       </c>
       <c r="K92" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Silicon.png</v>
       </c>
-    </row>
-    <row r="93" spans="1:11">
+      <c r="L92" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Silicon = config.get("enabledBlocks", "Silicon", true).getBoolean(true);</v>
+      </c>
+      <c r="N92" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Silicon = false;</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14">
       <c r="A93" t="s">
         <v>96</v>
       </c>
@@ -2957,23 +3694,31 @@
         <v>93</v>
       </c>
       <c r="D93" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _SilverBlock = new BlockBase("blockSilver");</v>
       </c>
       <c r="F93" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockSilver", new ItemStack(_SilverBlock, 1, 93));</v>
       </c>
       <c r="H93" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_SilverBlock);</v>
       </c>
       <c r="K93" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Silver.png</v>
       </c>
-    </row>
-    <row r="94" spans="1:11">
+      <c r="L93" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Silver = config.get("enabledBlocks", "Silver", true).getBoolean(true);</v>
+      </c>
+      <c r="N93" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Silver = false;</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14">
       <c r="A94" t="s">
         <v>97</v>
       </c>
@@ -2981,23 +3726,31 @@
         <v>94</v>
       </c>
       <c r="D94" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _SolderingAlloyBlock = new BlockBase("blockSolderingAlloy");</v>
       </c>
       <c r="F94" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockSolderingAlloy", new ItemStack(_SolderingAlloyBlock, 1, 94));</v>
       </c>
       <c r="H94" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_SolderingAlloyBlock);</v>
       </c>
       <c r="K94" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_SolderingAlloy.png</v>
       </c>
-    </row>
-    <row r="95" spans="1:11">
+      <c r="L94" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean SolderingAlloy = config.get("enabledBlocks", "SolderingAlloy", true).getBoolean(true);</v>
+      </c>
+      <c r="N94" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean SolderingAlloy = false;</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14">
       <c r="A95" t="s">
         <v>98</v>
       </c>
@@ -3005,23 +3758,31 @@
         <v>95</v>
       </c>
       <c r="D95" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _StainlessSteelBlock = new BlockBase("blockStainlessSteel");</v>
       </c>
       <c r="F95" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockStainlessSteel", new ItemStack(_StainlessSteelBlock, 1, 95));</v>
       </c>
       <c r="H95" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_StainlessSteelBlock);</v>
       </c>
       <c r="K95" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_StainlessSteel.png</v>
       </c>
-    </row>
-    <row r="96" spans="1:11">
+      <c r="L95" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean StainlessSteel = config.get("enabledBlocks", "StainlessSteel", true).getBoolean(true);</v>
+      </c>
+      <c r="N95" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean StainlessSteel = false;</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14">
       <c r="A96" t="s">
         <v>100</v>
       </c>
@@ -3029,23 +3790,31 @@
         <v>96</v>
       </c>
       <c r="D96" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _SteelMagneticBlock = new BlockBase("blockSteelMagnetic");</v>
       </c>
       <c r="F96" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockSteelMagnetic", new ItemStack(_SteelMagneticBlock, 1, 96));</v>
       </c>
       <c r="H96" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_SteelMagneticBlock);</v>
       </c>
       <c r="K96" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_SteelMagnetic.png</v>
       </c>
-    </row>
-    <row r="97" spans="1:11">
+      <c r="L96" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean SteelMagnetic = config.get("enabledBlocks", "SteelMagnetic", true).getBoolean(true);</v>
+      </c>
+      <c r="N96" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean SteelMagnetic = false;</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14">
       <c r="A97" t="s">
         <v>101</v>
       </c>
@@ -3053,23 +3822,31 @@
         <v>97</v>
       </c>
       <c r="D97" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _SteelBlock = new BlockBase("blockSteel");</v>
       </c>
       <c r="F97" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockSteel", new ItemStack(_SteelBlock, 1, 97));</v>
       </c>
       <c r="H97" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_SteelBlock);</v>
       </c>
       <c r="K97" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Steel.png</v>
       </c>
-    </row>
-    <row r="98" spans="1:11">
+      <c r="L97" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Steel = config.get("enabledBlocks", "Steel", true).getBoolean(true);</v>
+      </c>
+      <c r="N97" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Steel = false;</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14">
       <c r="A98" t="s">
         <v>102</v>
       </c>
@@ -3077,23 +3854,31 @@
         <v>98</v>
       </c>
       <c r="D98" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _SteeleafBlock = new BlockBase("blockSteeleaf");</v>
       </c>
       <c r="F98" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockSteeleaf", new ItemStack(_SteeleafBlock, 1, 98));</v>
       </c>
       <c r="H98" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_SteeleafBlock);</v>
       </c>
       <c r="K98" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Steeleaf.png</v>
       </c>
-    </row>
-    <row r="99" spans="1:11">
+      <c r="L98" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Steeleaf = config.get("enabledBlocks", "Steeleaf", true).getBoolean(true);</v>
+      </c>
+      <c r="N98" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Steeleaf = false;</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14">
       <c r="A99" t="s">
         <v>103</v>
       </c>
@@ -3101,23 +3886,31 @@
         <v>99</v>
       </c>
       <c r="D99" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _SterlingSilverBlock = new BlockBase("blockSterlingSilver");</v>
       </c>
       <c r="F99" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockSterlingSilver", new ItemStack(_SterlingSilverBlock, 1, 99));</v>
       </c>
       <c r="H99" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_SterlingSilverBlock);</v>
       </c>
       <c r="K99" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_SterlingSilver.png</v>
       </c>
-    </row>
-    <row r="100" spans="1:11">
+      <c r="L99" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean SterlingSilver = config.get("enabledBlocks", "SterlingSilver", true).getBoolean(true);</v>
+      </c>
+      <c r="N99" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean SterlingSilver = false;</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14">
       <c r="A100" t="s">
         <v>104</v>
       </c>
@@ -3125,23 +3918,31 @@
         <v>100</v>
       </c>
       <c r="D100" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _SunnariumBlock = new BlockBase("blockSunnarium");</v>
       </c>
       <c r="F100" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockSunnarium", new ItemStack(_SunnariumBlock, 1, 100));</v>
       </c>
       <c r="H100" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_SunnariumBlock);</v>
       </c>
       <c r="K100" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Sunnarium.png</v>
       </c>
-    </row>
-    <row r="101" spans="1:11">
+      <c r="L100" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Sunnarium = config.get("enabledBlocks", "Sunnarium", true).getBoolean(true);</v>
+      </c>
+      <c r="N100" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Sunnarium = false;</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14">
       <c r="A101" t="s">
         <v>105</v>
       </c>
@@ -3149,23 +3950,31 @@
         <v>101</v>
       </c>
       <c r="D101" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _TantalumBlock = new BlockBase("blockTantalum");</v>
       </c>
       <c r="F101" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockTantalum", new ItemStack(_TantalumBlock, 1, 101));</v>
       </c>
       <c r="H101" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_TantalumBlock);</v>
       </c>
       <c r="K101" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Tantalum.png</v>
       </c>
-    </row>
-    <row r="102" spans="1:11">
+      <c r="L101" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Tantalum = config.get("enabledBlocks", "Tantalum", true).getBoolean(true);</v>
+      </c>
+      <c r="N101" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Tantalum = false;</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14">
       <c r="A102" t="s">
         <v>106</v>
       </c>
@@ -3173,23 +3982,31 @@
         <v>102</v>
       </c>
       <c r="D102" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _TelluriumBlock = new BlockBase("blockTellurium");</v>
       </c>
       <c r="F102" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockTellurium", new ItemStack(_TelluriumBlock, 1, 102));</v>
       </c>
       <c r="H102" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_TelluriumBlock);</v>
       </c>
       <c r="K102" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Tellurium.png</v>
       </c>
-    </row>
-    <row r="103" spans="1:11">
+      <c r="L102" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Tellurium = config.get("enabledBlocks", "Tellurium", true).getBoolean(true);</v>
+      </c>
+      <c r="N102" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Tellurium = false;</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14">
       <c r="A103" t="s">
         <v>107</v>
       </c>
@@ -3197,23 +4014,31 @@
         <v>103</v>
       </c>
       <c r="D103" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _TerbiumBlock = new BlockBase("blockTerbium");</v>
       </c>
       <c r="F103" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockTerbium", new ItemStack(_TerbiumBlock, 1, 103));</v>
       </c>
       <c r="H103" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_TerbiumBlock);</v>
       </c>
       <c r="K103" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Terbium.png</v>
       </c>
-    </row>
-    <row r="104" spans="1:11">
+      <c r="L103" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Terbium = config.get("enabledBlocks", "Terbium", true).getBoolean(true);</v>
+      </c>
+      <c r="N103" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Terbium = false;</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14">
       <c r="A104" t="s">
         <v>108</v>
       </c>
@@ -3221,23 +4046,31 @@
         <v>104</v>
       </c>
       <c r="D104" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _ThaumiumBlock = new BlockBase("blockThaumium");</v>
       </c>
       <c r="F104" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockThaumium", new ItemStack(_ThaumiumBlock, 1, 104));</v>
       </c>
       <c r="H104" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_ThaumiumBlock);</v>
       </c>
       <c r="K104" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Thaumium.png</v>
       </c>
-    </row>
-    <row r="105" spans="1:11">
+      <c r="L104" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Thaumium = config.get("enabledBlocks", "Thaumium", true).getBoolean(true);</v>
+      </c>
+      <c r="N104" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Thaumium = false;</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14">
       <c r="A105" t="s">
         <v>109</v>
       </c>
@@ -3245,23 +4078,31 @@
         <v>105</v>
       </c>
       <c r="D105" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _ThoriumBlock = new BlockBase("blockThorium");</v>
       </c>
       <c r="F105" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockThorium", new ItemStack(_ThoriumBlock, 1, 105));</v>
       </c>
       <c r="H105" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_ThoriumBlock);</v>
       </c>
       <c r="K105" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Thorium.png</v>
       </c>
-    </row>
-    <row r="106" spans="1:11">
+      <c r="L105" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Thorium = config.get("enabledBlocks", "Thorium", true).getBoolean(true);</v>
+      </c>
+      <c r="N105" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Thorium = false;</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14">
       <c r="A106" t="s">
         <v>110</v>
       </c>
@@ -3269,23 +4110,31 @@
         <v>106</v>
       </c>
       <c r="D106" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _ThuliumBlock = new BlockBase("blockThulium");</v>
       </c>
       <c r="F106" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockThulium", new ItemStack(_ThuliumBlock, 1, 106));</v>
       </c>
       <c r="H106" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_ThuliumBlock);</v>
       </c>
       <c r="K106" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Thulium.png</v>
       </c>
-    </row>
-    <row r="107" spans="1:11">
+      <c r="L106" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Thulium = config.get("enabledBlocks", "Thulium", true).getBoolean(true);</v>
+      </c>
+      <c r="N106" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Thulium = false;</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14">
       <c r="A107" t="s">
         <v>111</v>
       </c>
@@ -3293,23 +4142,31 @@
         <v>107</v>
       </c>
       <c r="D107" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _TinAlloyBlock = new BlockBase("blockTinAlloy");</v>
       </c>
       <c r="F107" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockTinAlloy", new ItemStack(_TinAlloyBlock, 1, 107));</v>
       </c>
       <c r="H107" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_TinAlloyBlock);</v>
       </c>
       <c r="K107" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_TinAlloy.png</v>
       </c>
-    </row>
-    <row r="108" spans="1:11">
+      <c r="L107" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean TinAlloy = config.get("enabledBlocks", "TinAlloy", true).getBoolean(true);</v>
+      </c>
+      <c r="N107" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean TinAlloy = false;</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14">
       <c r="A108" t="s">
         <v>112</v>
       </c>
@@ -3317,23 +4174,31 @@
         <v>108</v>
       </c>
       <c r="D108" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _TinBlock = new BlockBase("blockTin");</v>
       </c>
       <c r="F108" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockTin", new ItemStack(_TinBlock, 1, 108));</v>
       </c>
       <c r="H108" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_TinBlock);</v>
       </c>
       <c r="K108" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Tin.png</v>
       </c>
-    </row>
-    <row r="109" spans="1:11">
+      <c r="L108" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Tin = config.get("enabledBlocks", "Tin", true).getBoolean(true);</v>
+      </c>
+      <c r="N108" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Tin = false;</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14">
       <c r="A109" t="s">
         <v>113</v>
       </c>
@@ -3341,23 +4206,31 @@
         <v>109</v>
       </c>
       <c r="D109" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _TitaniumBlock = new BlockBase("blockTitanium");</v>
       </c>
       <c r="F109" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockTitanium", new ItemStack(_TitaniumBlock, 1, 109));</v>
       </c>
       <c r="H109" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_TitaniumBlock);</v>
       </c>
       <c r="K109" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Titanium.png</v>
       </c>
-    </row>
-    <row r="110" spans="1:11">
+      <c r="L109" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Titanium = config.get("enabledBlocks", "Titanium", true).getBoolean(true);</v>
+      </c>
+      <c r="N109" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Titanium = false;</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14">
       <c r="A110" t="s">
         <v>114</v>
       </c>
@@ -3365,23 +4238,31 @@
         <v>110</v>
       </c>
       <c r="D110" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _TritaniumBlock = new BlockBase("blockTritanium");</v>
       </c>
       <c r="F110" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockTritanium", new ItemStack(_TritaniumBlock, 1, 110));</v>
       </c>
       <c r="H110" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_TritaniumBlock);</v>
       </c>
       <c r="K110" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Tritanium.png</v>
       </c>
-    </row>
-    <row r="111" spans="1:11">
+      <c r="L110" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Tritanium = config.get("enabledBlocks", "Tritanium", true).getBoolean(true);</v>
+      </c>
+      <c r="N110" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Tritanium = false;</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14">
       <c r="A111" t="s">
         <v>115</v>
       </c>
@@ -3389,23 +4270,31 @@
         <v>111</v>
       </c>
       <c r="D111" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _TungstenSteelBlock = new BlockBase("blockTungstenSteel");</v>
       </c>
       <c r="F111" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockTungstenSteel", new ItemStack(_TungstenSteelBlock, 1, 111));</v>
       </c>
       <c r="H111" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_TungstenSteelBlock);</v>
       </c>
       <c r="K111" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_TungstenSteel.png</v>
       </c>
-    </row>
-    <row r="112" spans="1:11">
+      <c r="L111" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean TungstenSteel = config.get("enabledBlocks", "TungstenSteel", true).getBoolean(true);</v>
+      </c>
+      <c r="N111" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean TungstenSteel = false;</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14">
       <c r="A112" t="s">
         <v>116</v>
       </c>
@@ -3413,23 +4302,31 @@
         <v>112</v>
       </c>
       <c r="D112" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _TungstenBlock = new BlockBase("blockTungsten");</v>
       </c>
       <c r="F112" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockTungsten", new ItemStack(_TungstenBlock, 1, 112));</v>
       </c>
       <c r="H112" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_TungstenBlock);</v>
       </c>
       <c r="K112" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Tungsten.png</v>
       </c>
-    </row>
-    <row r="113" spans="1:11">
+      <c r="L112" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Tungsten = config.get("enabledBlocks", "Tungsten", true).getBoolean(true);</v>
+      </c>
+      <c r="N112" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Tungsten = false;</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14">
       <c r="A113" t="s">
         <v>117</v>
       </c>
@@ -3437,23 +4334,31 @@
         <v>113</v>
       </c>
       <c r="D113" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _UltimetBlock = new BlockBase("blockUltimet");</v>
       </c>
       <c r="F113" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockUltimet", new ItemStack(_UltimetBlock, 1, 113));</v>
       </c>
       <c r="H113" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_UltimetBlock);</v>
       </c>
       <c r="K113" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Ultimet.png</v>
       </c>
-    </row>
-    <row r="114" spans="1:11">
+      <c r="L113" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Ultimet = config.get("enabledBlocks", "Ultimet", true).getBoolean(true);</v>
+      </c>
+      <c r="N113" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Ultimet = false;</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14">
       <c r="A114" t="s">
         <v>118</v>
       </c>
@@ -3461,23 +4366,31 @@
         <v>114</v>
       </c>
       <c r="D114" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _Uranium235Block = new BlockBase("blockUranium235");</v>
       </c>
       <c r="F114" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockUranium235", new ItemStack(_Uranium235Block, 1, 114));</v>
       </c>
       <c r="H114" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_Uranium235Block);</v>
       </c>
       <c r="K114" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Uranium235.png</v>
       </c>
-    </row>
-    <row r="115" spans="1:11">
+      <c r="L114" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Uranium235 = config.get("enabledBlocks", "Uranium235", true).getBoolean(true);</v>
+      </c>
+      <c r="N114" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Uranium235 = false;</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14">
       <c r="A115" t="s">
         <v>119</v>
       </c>
@@ -3485,23 +4398,31 @@
         <v>115</v>
       </c>
       <c r="D115" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _UraniumBlock = new BlockBase("blockUranium");</v>
       </c>
       <c r="F115" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockUranium", new ItemStack(_UraniumBlock, 1, 115));</v>
       </c>
       <c r="H115" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_UraniumBlock);</v>
       </c>
       <c r="K115" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Uranium.png</v>
       </c>
-    </row>
-    <row r="116" spans="1:11">
+      <c r="L115" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Uranium = config.get("enabledBlocks", "Uranium", true).getBoolean(true);</v>
+      </c>
+      <c r="N115" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Uranium = false;</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14">
       <c r="A116" t="s">
         <v>120</v>
       </c>
@@ -3509,23 +4430,31 @@
         <v>116</v>
       </c>
       <c r="D116" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _VanadiumGalliumBlock = new BlockBase("blockVanadiumGallium");</v>
       </c>
       <c r="F116" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockVanadiumGallium", new ItemStack(_VanadiumGalliumBlock, 1, 116));</v>
       </c>
       <c r="H116" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_VanadiumGalliumBlock);</v>
       </c>
       <c r="K116" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_VanadiumGallium.png</v>
       </c>
-    </row>
-    <row r="117" spans="1:11">
+      <c r="L116" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean VanadiumGallium = config.get("enabledBlocks", "VanadiumGallium", true).getBoolean(true);</v>
+      </c>
+      <c r="N116" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean VanadiumGallium = false;</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14">
       <c r="A117" t="s">
         <v>121</v>
       </c>
@@ -3533,23 +4462,31 @@
         <v>117</v>
       </c>
       <c r="D117" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _VanadiumBlock = new BlockBase("blockVanadium");</v>
       </c>
       <c r="F117" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockVanadium", new ItemStack(_VanadiumBlock, 1, 117));</v>
       </c>
       <c r="H117" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_VanadiumBlock);</v>
       </c>
       <c r="K117" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Vanadium.png</v>
       </c>
-    </row>
-    <row r="118" spans="1:11">
+      <c r="L117" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Vanadium = config.get("enabledBlocks", "Vanadium", true).getBoolean(true);</v>
+      </c>
+      <c r="N117" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Vanadium = false;</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14">
       <c r="A118" t="s">
         <v>122</v>
       </c>
@@ -3557,23 +4494,31 @@
         <v>118</v>
       </c>
       <c r="D118" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _WroughtIronBlock = new BlockBase("blockWroughtIron");</v>
       </c>
       <c r="F118" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockWroughtIron", new ItemStack(_WroughtIronBlock, 1, 118));</v>
       </c>
       <c r="H118" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_WroughtIronBlock);</v>
       </c>
       <c r="K118" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_WroughtIron.png</v>
       </c>
-    </row>
-    <row r="119" spans="1:11">
+      <c r="L118" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean WroughtIron = config.get("enabledBlocks", "WroughtIron", true).getBoolean(true);</v>
+      </c>
+      <c r="N118" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean WroughtIron = false;</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14">
       <c r="A119" t="s">
         <v>123</v>
       </c>
@@ -3581,23 +4526,31 @@
         <v>119</v>
       </c>
       <c r="D119" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _YtterbiumBlock = new BlockBase("blockYtterbium");</v>
       </c>
       <c r="F119" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockYtterbium", new ItemStack(_YtterbiumBlock, 1, 119));</v>
       </c>
       <c r="H119" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_YtterbiumBlock);</v>
       </c>
       <c r="K119" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Ytterbium.png</v>
       </c>
-    </row>
-    <row r="120" spans="1:11">
+      <c r="L119" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Ytterbium = config.get("enabledBlocks", "Ytterbium", true).getBoolean(true);</v>
+      </c>
+      <c r="N119" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Ytterbium = false;</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14">
       <c r="A120" t="s">
         <v>124</v>
       </c>
@@ -3605,23 +4558,31 @@
         <v>120</v>
       </c>
       <c r="D120" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _YttriumBariumCuprateBlock = new BlockBase("blockYttriumBariumCuprate");</v>
       </c>
       <c r="F120" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockYttriumBariumCuprate", new ItemStack(_YttriumBariumCuprateBlock, 1, 120));</v>
       </c>
       <c r="H120" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_YttriumBariumCuprateBlock);</v>
       </c>
       <c r="K120" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_YttriumBariumCuprate.png</v>
       </c>
-    </row>
-    <row r="121" spans="1:11">
+      <c r="L120" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean YttriumBariumCuprate = config.get("enabledBlocks", "YttriumBariumCuprate", true).getBoolean(true);</v>
+      </c>
+      <c r="N120" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean YttriumBariumCuprate = false;</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14">
       <c r="A121" t="s">
         <v>125</v>
       </c>
@@ -3629,23 +4590,31 @@
         <v>121</v>
       </c>
       <c r="D121" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _YttriumBlock = new BlockBase("blockYttrium");</v>
       </c>
       <c r="F121" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockYttrium", new ItemStack(_YttriumBlock, 1, 121));</v>
       </c>
       <c r="H121" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_YttriumBlock);</v>
       </c>
       <c r="K121" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Yttrium.png</v>
       </c>
-    </row>
-    <row r="122" spans="1:11">
+      <c r="L121" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Yttrium = config.get("enabledBlocks", "Yttrium", true).getBoolean(true);</v>
+      </c>
+      <c r="N121" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Yttrium = false;</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14">
       <c r="A122" t="s">
         <v>126</v>
       </c>
@@ -3653,23 +4622,31 @@
         <v>122</v>
       </c>
       <c r="D122" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _ZincBlock = new BlockBase("blockZinc");</v>
       </c>
       <c r="F122" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockZinc", new ItemStack(_ZincBlock, 1, 122));</v>
       </c>
       <c r="H122" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_ZincBlock);</v>
       </c>
       <c r="K122" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Zinc.png</v>
       </c>
-    </row>
-    <row r="123" spans="1:11">
+      <c r="L122" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Zinc = config.get("enabledBlocks", "Zinc", true).getBoolean(true);</v>
+      </c>
+      <c r="N122" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Zinc = false;</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14">
       <c r="A123" t="s">
         <v>35</v>
       </c>
@@ -3677,23 +4654,31 @@
         <v>123</v>
       </c>
       <c r="D123" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _FieryBloodBlock = new BlockBase("blockFieryBlood");</v>
       </c>
       <c r="F123" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockFieryBlood", new ItemStack(_FieryBloodBlock, 1, 123));</v>
       </c>
       <c r="H123" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_FieryBloodBlock);</v>
       </c>
       <c r="K123" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_FieryBlood.png</v>
       </c>
-    </row>
-    <row r="124" spans="1:11">
+      <c r="L123" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean FieryBlood = config.get("enabledBlocks", "FieryBlood", true).getBoolean(true);</v>
+      </c>
+      <c r="N123" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean FieryBlood = false;</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14">
       <c r="A124" t="s">
         <v>58</v>
       </c>
@@ -3701,23 +4686,31 @@
         <v>124</v>
       </c>
       <c r="D124" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _MeatRawBlock = new BlockBase("blockMeatRaw");</v>
       </c>
       <c r="F124" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockMeatRaw", new ItemStack(_MeatRawBlock, 1, 124));</v>
       </c>
       <c r="H124" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_MeatRawBlock);</v>
       </c>
       <c r="K124" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_MeatRaw.png</v>
       </c>
-    </row>
-    <row r="125" spans="1:11">
+      <c r="L124" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean MeatRaw = config.get("enabledBlocks", "MeatRaw", true).getBoolean(true);</v>
+      </c>
+      <c r="N124" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean MeatRaw = false;</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14">
       <c r="A125" t="s">
         <v>80</v>
       </c>
@@ -3725,23 +4718,31 @@
         <v>125</v>
       </c>
       <c r="D125" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _PlasticBlock = new BlockBase("blockPlastic");</v>
       </c>
       <c r="F125" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockPlastic", new ItemStack(_PlasticBlock, 1, 125));</v>
       </c>
       <c r="H125" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_PlasticBlock);</v>
       </c>
       <c r="K125" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Plastic.png</v>
       </c>
-    </row>
-    <row r="126" spans="1:11">
+      <c r="L125" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Plastic = config.get("enabledBlocks", "Plastic", true).getBoolean(true);</v>
+      </c>
+      <c r="N125" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Plastic = false;</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14">
       <c r="A126" t="s">
         <v>89</v>
       </c>
@@ -3749,23 +4750,31 @@
         <v>126</v>
       </c>
       <c r="D126" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _RubberBlock = new BlockBase("blockRubber");</v>
       </c>
       <c r="F126" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockRubber", new ItemStack(_RubberBlock, 1, 126));</v>
       </c>
       <c r="H126" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_RubberBlock);</v>
       </c>
       <c r="K126" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_Rubber.png</v>
       </c>
-    </row>
-    <row r="127" spans="1:11">
+      <c r="L126" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean Rubber = config.get("enabledBlocks", "Rubber", true).getBoolean(true);</v>
+      </c>
+      <c r="N126" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean Rubber = false;</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14">
       <c r="A127" t="s">
         <v>99</v>
       </c>
@@ -3773,20 +4782,28 @@
         <v>127</v>
       </c>
       <c r="D127" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public static Block _SteelLeafBlock = new BlockBase("blockSteelLeaf");</v>
       </c>
       <c r="F127" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>OreDictionary.registerOre("blockSteelLeaf", new ItemStack(_SteelLeafBlock, 1, 127));</v>
       </c>
       <c r="H127" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>RegisterHelper.registerBlock(_SteelLeafBlock);</v>
       </c>
       <c r="K127" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>copy dummy.png Block_SteelLeaf.png</v>
+      </c>
+      <c r="L127" t="str">
+        <f t="shared" si="10"/>
+        <v>public static boolean SteelLeaf = config.get("enabledBlocks", "SteelLeaf", true).getBoolean(true);</v>
+      </c>
+      <c r="N127" t="str">
+        <f t="shared" si="11"/>
+        <v>public static boolean SteelLeaf = false;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>